<commit_message>
Commit roteiro de teste atualizado_v02
</commit_message>
<xml_diff>
--- a/Roteiro_Teste_Selecao.xlsx
+++ b/Roteiro_Teste_Selecao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo.chen/automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5ECD3F-9E87-E94E-8D91-CBD8E784323C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D64D335-23FE-9C42-9D8C-DE5AF0DDACC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" tabRatio="639" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Evidences" sheetId="7" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cenários!$A$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cenários!$A$1:$G$6</definedName>
     <definedName name="_Toc391893800" localSheetId="2">Evidences!$C$5</definedName>
     <definedName name="_Toc391893801" localSheetId="2">Evidences!$C$10</definedName>
     <definedName name="_Toc391893802" localSheetId="2">Evidences!$C$28</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="78">
   <si>
     <t>This document shall be approved when all scenarios tested are acceptable for moving into Productive Environment.</t>
   </si>
@@ -379,11 +379,45 @@
 4.Nenhuma ação é exibida</t>
   </si>
   <si>
-    <t>Cenário 01 - Selecionar produto com sucesso</t>
+    <t>"Produto utilizado: "controle remoto do  papai noel"
+Url: https://magazineluiza.com.br"</t>
   </si>
   <si>
-    <t>"Produto utilizado: "controle remoto do  papai noel"
-Url: https://magazineluiza.com.br"</t>
+    <t>Cenário 01 - Selecionar produto por categoria</t>
+  </si>
+  <si>
+    <t>Cenário 02 - Selecinar produto por busca</t>
+  </si>
+  <si>
+    <t>Url: https://magazineluiza.com.br</t>
+  </si>
+  <si>
+    <t>1. Acessar o site da Magazine Luiza
+2. Na opção "Todos os departamentos" selecionar "Ferramentas"
+3. Selecionar o primeiro produto da lista
+4. Validar que o produtos</t>
+  </si>
+  <si>
+    <t>1. Acessar o site da Magazine Luiza
+2. No campo de busca inserir o produto desejado
+3. Clicar na "Lupa" para realizar a busca do produto
+4. Validar resultado após a busca
+5. Selecionar o produto para compra
+6. Validar a tela de produtos</t>
+  </si>
+  <si>
+    <t>1. Site aberto com sucesso
+2. A seção de ferramntas é apresentada com sucesso
+3. Tela de produtos é exibida com sucesso
+4.Tela de produtos validada com sucesso</t>
+  </si>
+  <si>
+    <t>1. Site aberto com sucesso
+2. Produto inserido com sucesso no campo de busca
+3. Botão "Lupa" foi clicado com sucesso
+4. Produto inserido no campo busca foi validado com sucesso e está presente na tela
+5. Produto selecionado com sucesso e a tela e produtos é exibida
+6. Tela de produtos validada com sucesso</t>
   </si>
 </sst>
 </file>
@@ -394,16 +428,9 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -624,7 +651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1008,17 +1035,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1027,80 +1043,80 @@
   </borders>
   <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1114,62 +1130,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1179,78 +1195,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1262,19 +1266,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1283,55 +1278,58 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1896,58 +1894,58 @@
       <c r="P12" s="20"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62" t="s">
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="67" t="s">
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="65"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="61"/>
     </row>
     <row r="14" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="66"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="62"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
       <c r="H15" s="22" t="s">
         <v>16</v>
       </c>
@@ -1965,10 +1963,10 @@
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="71"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
       <c r="H16" s="18" t="s">
         <v>17</v>
       </c>
@@ -1986,10 +1984,10 @@
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="11"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
       <c r="H17" s="18" t="s">
         <v>19</v>
       </c>
@@ -2007,10 +2005,10 @@
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="71"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="18"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -2024,10 +2022,10 @@
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="71"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="18"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -2041,10 +2039,10 @@
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="71"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="18"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -2058,10 +2056,10 @@
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="71"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="18"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -2075,10 +2073,10 @@
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="71"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="18"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -2092,10 +2090,10 @@
     <row r="23" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="74"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
       <c r="H23" s="4"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -2201,46 +2199,46 @@
       <c r="P30" s="20"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62" t="s">
+      <c r="C31" s="58"/>
+      <c r="D31" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="67" t="s">
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="65"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="61"/>
     </row>
     <row r="32" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="63"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="66"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="62"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
@@ -2490,46 +2488,46 @@
       <c r="P48" s="20"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62" t="s">
+      <c r="C49" s="58"/>
+      <c r="D49" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="67" t="s">
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="62" t="s">
+      <c r="I49" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
-      <c r="L49" s="62"/>
-      <c r="M49" s="62"/>
-      <c r="N49" s="62"/>
-      <c r="O49" s="62"/>
-      <c r="P49" s="65"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
+      <c r="P49" s="61"/>
     </row>
     <row r="50" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="63"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="64"/>
-      <c r="M50" s="64"/>
-      <c r="N50" s="64"/>
-      <c r="O50" s="64"/>
-      <c r="P50" s="66"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="60"/>
+      <c r="M50" s="60"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="62"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
@@ -2779,46 +2777,46 @@
       <c r="P66" s="20"/>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B67" s="61" t="s">
+      <c r="B67" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="62"/>
-      <c r="D67" s="62" t="s">
+      <c r="C67" s="58"/>
+      <c r="D67" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="67" t="s">
+      <c r="E67" s="58"/>
+      <c r="F67" s="58"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I67" s="62" t="s">
+      <c r="I67" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
-      <c r="L67" s="62"/>
-      <c r="M67" s="62"/>
-      <c r="N67" s="62"/>
-      <c r="O67" s="62"/>
-      <c r="P67" s="65"/>
+      <c r="J67" s="58"/>
+      <c r="K67" s="58"/>
+      <c r="L67" s="58"/>
+      <c r="M67" s="58"/>
+      <c r="N67" s="58"/>
+      <c r="O67" s="58"/>
+      <c r="P67" s="61"/>
     </row>
     <row r="68" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="63"/>
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="66"/>
-      <c r="H68" s="68"/>
-      <c r="I68" s="64"/>
-      <c r="J68" s="64"/>
-      <c r="K68" s="64"/>
-      <c r="L68" s="64"/>
-      <c r="M68" s="64"/>
-      <c r="N68" s="64"/>
-      <c r="O68" s="64"/>
-      <c r="P68" s="66"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="60"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="60"/>
+      <c r="J68" s="60"/>
+      <c r="K68" s="60"/>
+      <c r="L68" s="60"/>
+      <c r="M68" s="60"/>
+      <c r="N68" s="60"/>
+      <c r="O68" s="60"/>
+      <c r="P68" s="62"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B69" s="5"/>
@@ -3068,46 +3066,46 @@
       <c r="P84" s="20"/>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B85" s="61" t="s">
+      <c r="B85" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="62"/>
-      <c r="D85" s="62" t="s">
+      <c r="C85" s="58"/>
+      <c r="D85" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E85" s="62"/>
-      <c r="F85" s="62"/>
-      <c r="G85" s="65"/>
-      <c r="H85" s="67" t="s">
+      <c r="E85" s="58"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I85" s="62" t="s">
+      <c r="I85" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J85" s="62"/>
-      <c r="K85" s="62"/>
-      <c r="L85" s="62"/>
-      <c r="M85" s="62"/>
-      <c r="N85" s="62"/>
-      <c r="O85" s="62"/>
-      <c r="P85" s="65"/>
+      <c r="J85" s="58"/>
+      <c r="K85" s="58"/>
+      <c r="L85" s="58"/>
+      <c r="M85" s="58"/>
+      <c r="N85" s="58"/>
+      <c r="O85" s="58"/>
+      <c r="P85" s="61"/>
     </row>
     <row r="86" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="63"/>
-      <c r="C86" s="64"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="66"/>
-      <c r="H86" s="68"/>
-      <c r="I86" s="64"/>
-      <c r="J86" s="64"/>
-      <c r="K86" s="64"/>
-      <c r="L86" s="64"/>
-      <c r="M86" s="64"/>
-      <c r="N86" s="64"/>
-      <c r="O86" s="64"/>
-      <c r="P86" s="66"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="60"/>
+      <c r="D86" s="60"/>
+      <c r="E86" s="60"/>
+      <c r="F86" s="60"/>
+      <c r="G86" s="62"/>
+      <c r="H86" s="64"/>
+      <c r="I86" s="60"/>
+      <c r="J86" s="60"/>
+      <c r="K86" s="60"/>
+      <c r="L86" s="60"/>
+      <c r="M86" s="60"/>
+      <c r="N86" s="60"/>
+      <c r="O86" s="60"/>
+      <c r="P86" s="62"/>
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B87" s="5"/>
@@ -3357,46 +3355,46 @@
       <c r="P102" s="20"/>
     </row>
     <row r="103" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B103" s="61" t="s">
+      <c r="B103" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C103" s="62"/>
-      <c r="D103" s="62" t="s">
+      <c r="C103" s="58"/>
+      <c r="D103" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E103" s="62"/>
-      <c r="F103" s="62"/>
-      <c r="G103" s="65"/>
-      <c r="H103" s="67" t="s">
+      <c r="E103" s="58"/>
+      <c r="F103" s="58"/>
+      <c r="G103" s="61"/>
+      <c r="H103" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I103" s="62" t="s">
+      <c r="I103" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J103" s="62"/>
-      <c r="K103" s="62"/>
-      <c r="L103" s="62"/>
-      <c r="M103" s="62"/>
-      <c r="N103" s="62"/>
-      <c r="O103" s="62"/>
-      <c r="P103" s="65"/>
+      <c r="J103" s="58"/>
+      <c r="K103" s="58"/>
+      <c r="L103" s="58"/>
+      <c r="M103" s="58"/>
+      <c r="N103" s="58"/>
+      <c r="O103" s="58"/>
+      <c r="P103" s="61"/>
     </row>
     <row r="104" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="63"/>
-      <c r="C104" s="64"/>
-      <c r="D104" s="64"/>
-      <c r="E104" s="64"/>
-      <c r="F104" s="64"/>
-      <c r="G104" s="66"/>
-      <c r="H104" s="68"/>
-      <c r="I104" s="64"/>
-      <c r="J104" s="64"/>
-      <c r="K104" s="64"/>
-      <c r="L104" s="64"/>
-      <c r="M104" s="64"/>
-      <c r="N104" s="64"/>
-      <c r="O104" s="64"/>
-      <c r="P104" s="66"/>
+      <c r="B104" s="59"/>
+      <c r="C104" s="60"/>
+      <c r="D104" s="60"/>
+      <c r="E104" s="60"/>
+      <c r="F104" s="60"/>
+      <c r="G104" s="62"/>
+      <c r="H104" s="64"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="60"/>
+      <c r="K104" s="60"/>
+      <c r="L104" s="60"/>
+      <c r="M104" s="60"/>
+      <c r="N104" s="60"/>
+      <c r="O104" s="60"/>
+      <c r="P104" s="62"/>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B105" s="5"/>
@@ -3646,46 +3644,46 @@
       <c r="P120" s="20"/>
     </row>
     <row r="121" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B121" s="61" t="s">
+      <c r="B121" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C121" s="62"/>
-      <c r="D121" s="62" t="s">
+      <c r="C121" s="58"/>
+      <c r="D121" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E121" s="62"/>
-      <c r="F121" s="62"/>
-      <c r="G121" s="65"/>
-      <c r="H121" s="67" t="s">
+      <c r="E121" s="58"/>
+      <c r="F121" s="58"/>
+      <c r="G121" s="61"/>
+      <c r="H121" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I121" s="62" t="s">
+      <c r="I121" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J121" s="62"/>
-      <c r="K121" s="62"/>
-      <c r="L121" s="62"/>
-      <c r="M121" s="62"/>
-      <c r="N121" s="62"/>
-      <c r="O121" s="62"/>
-      <c r="P121" s="65"/>
+      <c r="J121" s="58"/>
+      <c r="K121" s="58"/>
+      <c r="L121" s="58"/>
+      <c r="M121" s="58"/>
+      <c r="N121" s="58"/>
+      <c r="O121" s="58"/>
+      <c r="P121" s="61"/>
     </row>
     <row r="122" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="63"/>
-      <c r="C122" s="64"/>
-      <c r="D122" s="64"/>
-      <c r="E122" s="64"/>
-      <c r="F122" s="64"/>
-      <c r="G122" s="66"/>
-      <c r="H122" s="68"/>
-      <c r="I122" s="64"/>
-      <c r="J122" s="64"/>
-      <c r="K122" s="64"/>
-      <c r="L122" s="64"/>
-      <c r="M122" s="64"/>
-      <c r="N122" s="64"/>
-      <c r="O122" s="64"/>
-      <c r="P122" s="66"/>
+      <c r="B122" s="59"/>
+      <c r="C122" s="60"/>
+      <c r="D122" s="60"/>
+      <c r="E122" s="60"/>
+      <c r="F122" s="60"/>
+      <c r="G122" s="62"/>
+      <c r="H122" s="64"/>
+      <c r="I122" s="60"/>
+      <c r="J122" s="60"/>
+      <c r="K122" s="60"/>
+      <c r="L122" s="60"/>
+      <c r="M122" s="60"/>
+      <c r="N122" s="60"/>
+      <c r="O122" s="60"/>
+      <c r="P122" s="62"/>
     </row>
     <row r="123" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B123" s="5"/>
@@ -3935,46 +3933,46 @@
       <c r="P138" s="20"/>
     </row>
     <row r="139" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B139" s="61" t="s">
+      <c r="B139" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C139" s="62"/>
-      <c r="D139" s="62" t="s">
+      <c r="C139" s="58"/>
+      <c r="D139" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E139" s="62"/>
-      <c r="F139" s="62"/>
-      <c r="G139" s="65"/>
-      <c r="H139" s="67" t="s">
+      <c r="E139" s="58"/>
+      <c r="F139" s="58"/>
+      <c r="G139" s="61"/>
+      <c r="H139" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I139" s="62" t="s">
+      <c r="I139" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J139" s="62"/>
-      <c r="K139" s="62"/>
-      <c r="L139" s="62"/>
-      <c r="M139" s="62"/>
-      <c r="N139" s="62"/>
-      <c r="O139" s="62"/>
-      <c r="P139" s="65"/>
+      <c r="J139" s="58"/>
+      <c r="K139" s="58"/>
+      <c r="L139" s="58"/>
+      <c r="M139" s="58"/>
+      <c r="N139" s="58"/>
+      <c r="O139" s="58"/>
+      <c r="P139" s="61"/>
     </row>
     <row r="140" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="63"/>
-      <c r="C140" s="64"/>
-      <c r="D140" s="64"/>
-      <c r="E140" s="64"/>
-      <c r="F140" s="64"/>
-      <c r="G140" s="66"/>
-      <c r="H140" s="68"/>
-      <c r="I140" s="64"/>
-      <c r="J140" s="64"/>
-      <c r="K140" s="64"/>
-      <c r="L140" s="64"/>
-      <c r="M140" s="64"/>
-      <c r="N140" s="64"/>
-      <c r="O140" s="64"/>
-      <c r="P140" s="66"/>
+      <c r="B140" s="59"/>
+      <c r="C140" s="60"/>
+      <c r="D140" s="60"/>
+      <c r="E140" s="60"/>
+      <c r="F140" s="60"/>
+      <c r="G140" s="62"/>
+      <c r="H140" s="64"/>
+      <c r="I140" s="60"/>
+      <c r="J140" s="60"/>
+      <c r="K140" s="60"/>
+      <c r="L140" s="60"/>
+      <c r="M140" s="60"/>
+      <c r="N140" s="60"/>
+      <c r="O140" s="60"/>
+      <c r="P140" s="62"/>
     </row>
     <row r="141" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B141" s="5"/>
@@ -4224,46 +4222,46 @@
       <c r="P156" s="20"/>
     </row>
     <row r="157" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B157" s="61" t="s">
+      <c r="B157" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C157" s="62"/>
-      <c r="D157" s="62" t="s">
+      <c r="C157" s="58"/>
+      <c r="D157" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E157" s="62"/>
-      <c r="F157" s="62"/>
-      <c r="G157" s="65"/>
-      <c r="H157" s="67" t="s">
+      <c r="E157" s="58"/>
+      <c r="F157" s="58"/>
+      <c r="G157" s="61"/>
+      <c r="H157" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I157" s="62" t="s">
+      <c r="I157" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J157" s="62"/>
-      <c r="K157" s="62"/>
-      <c r="L157" s="62"/>
-      <c r="M157" s="62"/>
-      <c r="N157" s="62"/>
-      <c r="O157" s="62"/>
-      <c r="P157" s="65"/>
+      <c r="J157" s="58"/>
+      <c r="K157" s="58"/>
+      <c r="L157" s="58"/>
+      <c r="M157" s="58"/>
+      <c r="N157" s="58"/>
+      <c r="O157" s="58"/>
+      <c r="P157" s="61"/>
     </row>
     <row r="158" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="63"/>
-      <c r="C158" s="64"/>
-      <c r="D158" s="64"/>
-      <c r="E158" s="64"/>
-      <c r="F158" s="64"/>
-      <c r="G158" s="66"/>
-      <c r="H158" s="68"/>
-      <c r="I158" s="64"/>
-      <c r="J158" s="64"/>
-      <c r="K158" s="64"/>
-      <c r="L158" s="64"/>
-      <c r="M158" s="64"/>
-      <c r="N158" s="64"/>
-      <c r="O158" s="64"/>
-      <c r="P158" s="66"/>
+      <c r="B158" s="59"/>
+      <c r="C158" s="60"/>
+      <c r="D158" s="60"/>
+      <c r="E158" s="60"/>
+      <c r="F158" s="60"/>
+      <c r="G158" s="62"/>
+      <c r="H158" s="64"/>
+      <c r="I158" s="60"/>
+      <c r="J158" s="60"/>
+      <c r="K158" s="60"/>
+      <c r="L158" s="60"/>
+      <c r="M158" s="60"/>
+      <c r="N158" s="60"/>
+      <c r="O158" s="60"/>
+      <c r="P158" s="62"/>
     </row>
     <row r="159" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B159" s="5"/>
@@ -4513,46 +4511,46 @@
       <c r="P174" s="20"/>
     </row>
     <row r="175" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B175" s="61" t="s">
+      <c r="B175" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C175" s="62"/>
-      <c r="D175" s="62" t="s">
+      <c r="C175" s="58"/>
+      <c r="D175" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E175" s="62"/>
-      <c r="F175" s="62"/>
-      <c r="G175" s="65"/>
-      <c r="H175" s="67" t="s">
+      <c r="E175" s="58"/>
+      <c r="F175" s="58"/>
+      <c r="G175" s="61"/>
+      <c r="H175" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I175" s="62" t="s">
+      <c r="I175" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J175" s="62"/>
-      <c r="K175" s="62"/>
-      <c r="L175" s="62"/>
-      <c r="M175" s="62"/>
-      <c r="N175" s="62"/>
-      <c r="O175" s="62"/>
-      <c r="P175" s="65"/>
+      <c r="J175" s="58"/>
+      <c r="K175" s="58"/>
+      <c r="L175" s="58"/>
+      <c r="M175" s="58"/>
+      <c r="N175" s="58"/>
+      <c r="O175" s="58"/>
+      <c r="P175" s="61"/>
     </row>
     <row r="176" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="63"/>
-      <c r="C176" s="64"/>
-      <c r="D176" s="64"/>
-      <c r="E176" s="64"/>
-      <c r="F176" s="64"/>
-      <c r="G176" s="66"/>
-      <c r="H176" s="68"/>
-      <c r="I176" s="64"/>
-      <c r="J176" s="64"/>
-      <c r="K176" s="64"/>
-      <c r="L176" s="64"/>
-      <c r="M176" s="64"/>
-      <c r="N176" s="64"/>
-      <c r="O176" s="64"/>
-      <c r="P176" s="66"/>
+      <c r="B176" s="59"/>
+      <c r="C176" s="60"/>
+      <c r="D176" s="60"/>
+      <c r="E176" s="60"/>
+      <c r="F176" s="60"/>
+      <c r="G176" s="62"/>
+      <c r="H176" s="64"/>
+      <c r="I176" s="60"/>
+      <c r="J176" s="60"/>
+      <c r="K176" s="60"/>
+      <c r="L176" s="60"/>
+      <c r="M176" s="60"/>
+      <c r="N176" s="60"/>
+      <c r="O176" s="60"/>
+      <c r="P176" s="62"/>
     </row>
     <row r="177" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B177" s="5"/>
@@ -4802,46 +4800,46 @@
       <c r="P192" s="20"/>
     </row>
     <row r="193" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B193" s="61" t="s">
+      <c r="B193" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C193" s="62"/>
-      <c r="D193" s="62" t="s">
+      <c r="C193" s="58"/>
+      <c r="D193" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E193" s="62"/>
-      <c r="F193" s="62"/>
-      <c r="G193" s="65"/>
-      <c r="H193" s="67" t="s">
+      <c r="E193" s="58"/>
+      <c r="F193" s="58"/>
+      <c r="G193" s="61"/>
+      <c r="H193" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I193" s="62" t="s">
+      <c r="I193" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J193" s="62"/>
-      <c r="K193" s="62"/>
-      <c r="L193" s="62"/>
-      <c r="M193" s="62"/>
-      <c r="N193" s="62"/>
-      <c r="O193" s="62"/>
-      <c r="P193" s="65"/>
+      <c r="J193" s="58"/>
+      <c r="K193" s="58"/>
+      <c r="L193" s="58"/>
+      <c r="M193" s="58"/>
+      <c r="N193" s="58"/>
+      <c r="O193" s="58"/>
+      <c r="P193" s="61"/>
     </row>
     <row r="194" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="63"/>
-      <c r="C194" s="64"/>
-      <c r="D194" s="64"/>
-      <c r="E194" s="64"/>
-      <c r="F194" s="64"/>
-      <c r="G194" s="66"/>
-      <c r="H194" s="68"/>
-      <c r="I194" s="64"/>
-      <c r="J194" s="64"/>
-      <c r="K194" s="64"/>
-      <c r="L194" s="64"/>
-      <c r="M194" s="64"/>
-      <c r="N194" s="64"/>
-      <c r="O194" s="64"/>
-      <c r="P194" s="66"/>
+      <c r="B194" s="59"/>
+      <c r="C194" s="60"/>
+      <c r="D194" s="60"/>
+      <c r="E194" s="60"/>
+      <c r="F194" s="60"/>
+      <c r="G194" s="62"/>
+      <c r="H194" s="64"/>
+      <c r="I194" s="60"/>
+      <c r="J194" s="60"/>
+      <c r="K194" s="60"/>
+      <c r="L194" s="60"/>
+      <c r="M194" s="60"/>
+      <c r="N194" s="60"/>
+      <c r="O194" s="60"/>
+      <c r="P194" s="62"/>
     </row>
     <row r="195" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B195" s="5"/>
@@ -5091,46 +5089,46 @@
       <c r="P210" s="20"/>
     </row>
     <row r="211" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B211" s="61" t="s">
+      <c r="B211" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C211" s="62"/>
-      <c r="D211" s="62" t="s">
+      <c r="C211" s="58"/>
+      <c r="D211" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E211" s="62"/>
-      <c r="F211" s="62"/>
-      <c r="G211" s="65"/>
-      <c r="H211" s="67" t="s">
+      <c r="E211" s="58"/>
+      <c r="F211" s="58"/>
+      <c r="G211" s="61"/>
+      <c r="H211" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I211" s="62" t="s">
+      <c r="I211" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J211" s="62"/>
-      <c r="K211" s="62"/>
-      <c r="L211" s="62"/>
-      <c r="M211" s="62"/>
-      <c r="N211" s="62"/>
-      <c r="O211" s="62"/>
-      <c r="P211" s="65"/>
+      <c r="J211" s="58"/>
+      <c r="K211" s="58"/>
+      <c r="L211" s="58"/>
+      <c r="M211" s="58"/>
+      <c r="N211" s="58"/>
+      <c r="O211" s="58"/>
+      <c r="P211" s="61"/>
     </row>
     <row r="212" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="63"/>
-      <c r="C212" s="64"/>
-      <c r="D212" s="64"/>
-      <c r="E212" s="64"/>
-      <c r="F212" s="64"/>
-      <c r="G212" s="66"/>
-      <c r="H212" s="68"/>
-      <c r="I212" s="64"/>
-      <c r="J212" s="64"/>
-      <c r="K212" s="64"/>
-      <c r="L212" s="64"/>
-      <c r="M212" s="64"/>
-      <c r="N212" s="64"/>
-      <c r="O212" s="64"/>
-      <c r="P212" s="66"/>
+      <c r="B212" s="59"/>
+      <c r="C212" s="60"/>
+      <c r="D212" s="60"/>
+      <c r="E212" s="60"/>
+      <c r="F212" s="60"/>
+      <c r="G212" s="62"/>
+      <c r="H212" s="64"/>
+      <c r="I212" s="60"/>
+      <c r="J212" s="60"/>
+      <c r="K212" s="60"/>
+      <c r="L212" s="60"/>
+      <c r="M212" s="60"/>
+      <c r="N212" s="60"/>
+      <c r="O212" s="60"/>
+      <c r="P212" s="62"/>
     </row>
     <row r="213" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B213" s="5"/>
@@ -5380,46 +5378,46 @@
       <c r="P228" s="20"/>
     </row>
     <row r="229" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B229" s="61" t="s">
+      <c r="B229" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C229" s="62"/>
-      <c r="D229" s="62" t="s">
+      <c r="C229" s="58"/>
+      <c r="D229" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E229" s="62"/>
-      <c r="F229" s="62"/>
-      <c r="G229" s="65"/>
-      <c r="H229" s="67" t="s">
+      <c r="E229" s="58"/>
+      <c r="F229" s="58"/>
+      <c r="G229" s="61"/>
+      <c r="H229" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I229" s="62" t="s">
+      <c r="I229" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J229" s="62"/>
-      <c r="K229" s="62"/>
-      <c r="L229" s="62"/>
-      <c r="M229" s="62"/>
-      <c r="N229" s="62"/>
-      <c r="O229" s="62"/>
-      <c r="P229" s="65"/>
+      <c r="J229" s="58"/>
+      <c r="K229" s="58"/>
+      <c r="L229" s="58"/>
+      <c r="M229" s="58"/>
+      <c r="N229" s="58"/>
+      <c r="O229" s="58"/>
+      <c r="P229" s="61"/>
     </row>
     <row r="230" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="63"/>
-      <c r="C230" s="64"/>
-      <c r="D230" s="64"/>
-      <c r="E230" s="64"/>
-      <c r="F230" s="64"/>
-      <c r="G230" s="66"/>
-      <c r="H230" s="68"/>
-      <c r="I230" s="64"/>
-      <c r="J230" s="64"/>
-      <c r="K230" s="64"/>
-      <c r="L230" s="64"/>
-      <c r="M230" s="64"/>
-      <c r="N230" s="64"/>
-      <c r="O230" s="64"/>
-      <c r="P230" s="66"/>
+      <c r="B230" s="59"/>
+      <c r="C230" s="60"/>
+      <c r="D230" s="60"/>
+      <c r="E230" s="60"/>
+      <c r="F230" s="60"/>
+      <c r="G230" s="62"/>
+      <c r="H230" s="64"/>
+      <c r="I230" s="60"/>
+      <c r="J230" s="60"/>
+      <c r="K230" s="60"/>
+      <c r="L230" s="60"/>
+      <c r="M230" s="60"/>
+      <c r="N230" s="60"/>
+      <c r="O230" s="60"/>
+      <c r="P230" s="62"/>
     </row>
     <row r="231" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B231" s="5"/>
@@ -5669,46 +5667,46 @@
       <c r="P246" s="20"/>
     </row>
     <row r="247" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B247" s="61" t="s">
+      <c r="B247" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C247" s="62"/>
-      <c r="D247" s="62" t="s">
+      <c r="C247" s="58"/>
+      <c r="D247" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E247" s="62"/>
-      <c r="F247" s="62"/>
-      <c r="G247" s="65"/>
-      <c r="H247" s="67" t="s">
+      <c r="E247" s="58"/>
+      <c r="F247" s="58"/>
+      <c r="G247" s="61"/>
+      <c r="H247" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I247" s="62" t="s">
+      <c r="I247" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J247" s="62"/>
-      <c r="K247" s="62"/>
-      <c r="L247" s="62"/>
-      <c r="M247" s="62"/>
-      <c r="N247" s="62"/>
-      <c r="O247" s="62"/>
-      <c r="P247" s="65"/>
+      <c r="J247" s="58"/>
+      <c r="K247" s="58"/>
+      <c r="L247" s="58"/>
+      <c r="M247" s="58"/>
+      <c r="N247" s="58"/>
+      <c r="O247" s="58"/>
+      <c r="P247" s="61"/>
     </row>
     <row r="248" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="63"/>
-      <c r="C248" s="64"/>
-      <c r="D248" s="64"/>
-      <c r="E248" s="64"/>
-      <c r="F248" s="64"/>
-      <c r="G248" s="66"/>
-      <c r="H248" s="68"/>
-      <c r="I248" s="64"/>
-      <c r="J248" s="64"/>
-      <c r="K248" s="64"/>
-      <c r="L248" s="64"/>
-      <c r="M248" s="64"/>
-      <c r="N248" s="64"/>
-      <c r="O248" s="64"/>
-      <c r="P248" s="66"/>
+      <c r="B248" s="59"/>
+      <c r="C248" s="60"/>
+      <c r="D248" s="60"/>
+      <c r="E248" s="60"/>
+      <c r="F248" s="60"/>
+      <c r="G248" s="62"/>
+      <c r="H248" s="64"/>
+      <c r="I248" s="60"/>
+      <c r="J248" s="60"/>
+      <c r="K248" s="60"/>
+      <c r="L248" s="60"/>
+      <c r="M248" s="60"/>
+      <c r="N248" s="60"/>
+      <c r="O248" s="60"/>
+      <c r="P248" s="62"/>
     </row>
     <row r="249" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B249" s="5"/>
@@ -5958,46 +5956,46 @@
       <c r="P264" s="20"/>
     </row>
     <row r="265" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B265" s="61" t="s">
+      <c r="B265" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C265" s="62"/>
-      <c r="D265" s="62" t="s">
+      <c r="C265" s="58"/>
+      <c r="D265" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E265" s="62"/>
-      <c r="F265" s="62"/>
-      <c r="G265" s="65"/>
-      <c r="H265" s="67" t="s">
+      <c r="E265" s="58"/>
+      <c r="F265" s="58"/>
+      <c r="G265" s="61"/>
+      <c r="H265" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I265" s="62" t="s">
+      <c r="I265" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J265" s="62"/>
-      <c r="K265" s="62"/>
-      <c r="L265" s="62"/>
-      <c r="M265" s="62"/>
-      <c r="N265" s="62"/>
-      <c r="O265" s="62"/>
-      <c r="P265" s="65"/>
+      <c r="J265" s="58"/>
+      <c r="K265" s="58"/>
+      <c r="L265" s="58"/>
+      <c r="M265" s="58"/>
+      <c r="N265" s="58"/>
+      <c r="O265" s="58"/>
+      <c r="P265" s="61"/>
     </row>
     <row r="266" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="63"/>
-      <c r="C266" s="64"/>
-      <c r="D266" s="64"/>
-      <c r="E266" s="64"/>
-      <c r="F266" s="64"/>
-      <c r="G266" s="66"/>
-      <c r="H266" s="68"/>
-      <c r="I266" s="64"/>
-      <c r="J266" s="64"/>
-      <c r="K266" s="64"/>
-      <c r="L266" s="64"/>
-      <c r="M266" s="64"/>
-      <c r="N266" s="64"/>
-      <c r="O266" s="64"/>
-      <c r="P266" s="66"/>
+      <c r="B266" s="59"/>
+      <c r="C266" s="60"/>
+      <c r="D266" s="60"/>
+      <c r="E266" s="60"/>
+      <c r="F266" s="60"/>
+      <c r="G266" s="62"/>
+      <c r="H266" s="64"/>
+      <c r="I266" s="60"/>
+      <c r="J266" s="60"/>
+      <c r="K266" s="60"/>
+      <c r="L266" s="60"/>
+      <c r="M266" s="60"/>
+      <c r="N266" s="60"/>
+      <c r="O266" s="60"/>
+      <c r="P266" s="62"/>
     </row>
     <row r="267" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B267" s="5"/>
@@ -6247,46 +6245,46 @@
       <c r="P282" s="20"/>
     </row>
     <row r="283" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B283" s="61" t="s">
+      <c r="B283" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C283" s="62"/>
-      <c r="D283" s="62" t="s">
+      <c r="C283" s="58"/>
+      <c r="D283" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E283" s="62"/>
-      <c r="F283" s="62"/>
-      <c r="G283" s="65"/>
-      <c r="H283" s="67" t="s">
+      <c r="E283" s="58"/>
+      <c r="F283" s="58"/>
+      <c r="G283" s="61"/>
+      <c r="H283" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I283" s="62" t="s">
+      <c r="I283" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J283" s="62"/>
-      <c r="K283" s="62"/>
-      <c r="L283" s="62"/>
-      <c r="M283" s="62"/>
-      <c r="N283" s="62"/>
-      <c r="O283" s="62"/>
-      <c r="P283" s="65"/>
+      <c r="J283" s="58"/>
+      <c r="K283" s="58"/>
+      <c r="L283" s="58"/>
+      <c r="M283" s="58"/>
+      <c r="N283" s="58"/>
+      <c r="O283" s="58"/>
+      <c r="P283" s="61"/>
     </row>
     <row r="284" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="63"/>
-      <c r="C284" s="64"/>
-      <c r="D284" s="64"/>
-      <c r="E284" s="64"/>
-      <c r="F284" s="64"/>
-      <c r="G284" s="66"/>
-      <c r="H284" s="68"/>
-      <c r="I284" s="64"/>
-      <c r="J284" s="64"/>
-      <c r="K284" s="64"/>
-      <c r="L284" s="64"/>
-      <c r="M284" s="64"/>
-      <c r="N284" s="64"/>
-      <c r="O284" s="64"/>
-      <c r="P284" s="66"/>
+      <c r="B284" s="59"/>
+      <c r="C284" s="60"/>
+      <c r="D284" s="60"/>
+      <c r="E284" s="60"/>
+      <c r="F284" s="60"/>
+      <c r="G284" s="62"/>
+      <c r="H284" s="64"/>
+      <c r="I284" s="60"/>
+      <c r="J284" s="60"/>
+      <c r="K284" s="60"/>
+      <c r="L284" s="60"/>
+      <c r="M284" s="60"/>
+      <c r="N284" s="60"/>
+      <c r="O284" s="60"/>
+      <c r="P284" s="62"/>
     </row>
     <row r="285" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B285" s="5"/>
@@ -6536,46 +6534,46 @@
       <c r="P300" s="20"/>
     </row>
     <row r="301" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B301" s="61" t="s">
+      <c r="B301" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C301" s="62"/>
-      <c r="D301" s="62" t="s">
+      <c r="C301" s="58"/>
+      <c r="D301" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E301" s="62"/>
-      <c r="F301" s="62"/>
-      <c r="G301" s="65"/>
-      <c r="H301" s="67" t="s">
+      <c r="E301" s="58"/>
+      <c r="F301" s="58"/>
+      <c r="G301" s="61"/>
+      <c r="H301" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I301" s="62" t="s">
+      <c r="I301" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J301" s="62"/>
-      <c r="K301" s="62"/>
-      <c r="L301" s="62"/>
-      <c r="M301" s="62"/>
-      <c r="N301" s="62"/>
-      <c r="O301" s="62"/>
-      <c r="P301" s="65"/>
+      <c r="J301" s="58"/>
+      <c r="K301" s="58"/>
+      <c r="L301" s="58"/>
+      <c r="M301" s="58"/>
+      <c r="N301" s="58"/>
+      <c r="O301" s="58"/>
+      <c r="P301" s="61"/>
     </row>
     <row r="302" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B302" s="63"/>
-      <c r="C302" s="64"/>
-      <c r="D302" s="64"/>
-      <c r="E302" s="64"/>
-      <c r="F302" s="64"/>
-      <c r="G302" s="66"/>
-      <c r="H302" s="68"/>
-      <c r="I302" s="64"/>
-      <c r="J302" s="64"/>
-      <c r="K302" s="64"/>
-      <c r="L302" s="64"/>
-      <c r="M302" s="64"/>
-      <c r="N302" s="64"/>
-      <c r="O302" s="64"/>
-      <c r="P302" s="66"/>
+      <c r="B302" s="59"/>
+      <c r="C302" s="60"/>
+      <c r="D302" s="60"/>
+      <c r="E302" s="60"/>
+      <c r="F302" s="60"/>
+      <c r="G302" s="62"/>
+      <c r="H302" s="64"/>
+      <c r="I302" s="60"/>
+      <c r="J302" s="60"/>
+      <c r="K302" s="60"/>
+      <c r="L302" s="60"/>
+      <c r="M302" s="60"/>
+      <c r="N302" s="60"/>
+      <c r="O302" s="60"/>
+      <c r="P302" s="62"/>
     </row>
     <row r="303" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B303" s="5"/>
@@ -6825,46 +6823,46 @@
       <c r="P318" s="20"/>
     </row>
     <row r="319" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B319" s="61" t="s">
+      <c r="B319" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C319" s="62"/>
-      <c r="D319" s="62" t="s">
+      <c r="C319" s="58"/>
+      <c r="D319" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E319" s="62"/>
-      <c r="F319" s="62"/>
-      <c r="G319" s="65"/>
-      <c r="H319" s="67" t="s">
+      <c r="E319" s="58"/>
+      <c r="F319" s="58"/>
+      <c r="G319" s="61"/>
+      <c r="H319" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I319" s="62" t="s">
+      <c r="I319" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J319" s="62"/>
-      <c r="K319" s="62"/>
-      <c r="L319" s="62"/>
-      <c r="M319" s="62"/>
-      <c r="N319" s="62"/>
-      <c r="O319" s="62"/>
-      <c r="P319" s="65"/>
+      <c r="J319" s="58"/>
+      <c r="K319" s="58"/>
+      <c r="L319" s="58"/>
+      <c r="M319" s="58"/>
+      <c r="N319" s="58"/>
+      <c r="O319" s="58"/>
+      <c r="P319" s="61"/>
     </row>
     <row r="320" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B320" s="63"/>
-      <c r="C320" s="64"/>
-      <c r="D320" s="64"/>
-      <c r="E320" s="64"/>
-      <c r="F320" s="64"/>
-      <c r="G320" s="66"/>
-      <c r="H320" s="68"/>
-      <c r="I320" s="64"/>
-      <c r="J320" s="64"/>
-      <c r="K320" s="64"/>
-      <c r="L320" s="64"/>
-      <c r="M320" s="64"/>
-      <c r="N320" s="64"/>
-      <c r="O320" s="64"/>
-      <c r="P320" s="66"/>
+      <c r="B320" s="59"/>
+      <c r="C320" s="60"/>
+      <c r="D320" s="60"/>
+      <c r="E320" s="60"/>
+      <c r="F320" s="60"/>
+      <c r="G320" s="62"/>
+      <c r="H320" s="64"/>
+      <c r="I320" s="60"/>
+      <c r="J320" s="60"/>
+      <c r="K320" s="60"/>
+      <c r="L320" s="60"/>
+      <c r="M320" s="60"/>
+      <c r="N320" s="60"/>
+      <c r="O320" s="60"/>
+      <c r="P320" s="62"/>
     </row>
     <row r="321" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B321" s="5"/>
@@ -7114,46 +7112,46 @@
       <c r="P336" s="20"/>
     </row>
     <row r="337" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B337" s="61" t="s">
+      <c r="B337" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C337" s="62"/>
-      <c r="D337" s="62" t="s">
+      <c r="C337" s="58"/>
+      <c r="D337" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E337" s="62"/>
-      <c r="F337" s="62"/>
-      <c r="G337" s="65"/>
-      <c r="H337" s="67" t="s">
+      <c r="E337" s="58"/>
+      <c r="F337" s="58"/>
+      <c r="G337" s="61"/>
+      <c r="H337" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I337" s="62" t="s">
+      <c r="I337" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J337" s="62"/>
-      <c r="K337" s="62"/>
-      <c r="L337" s="62"/>
-      <c r="M337" s="62"/>
-      <c r="N337" s="62"/>
-      <c r="O337" s="62"/>
-      <c r="P337" s="65"/>
+      <c r="J337" s="58"/>
+      <c r="K337" s="58"/>
+      <c r="L337" s="58"/>
+      <c r="M337" s="58"/>
+      <c r="N337" s="58"/>
+      <c r="O337" s="58"/>
+      <c r="P337" s="61"/>
     </row>
     <row r="338" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B338" s="63"/>
-      <c r="C338" s="64"/>
-      <c r="D338" s="64"/>
-      <c r="E338" s="64"/>
-      <c r="F338" s="64"/>
-      <c r="G338" s="66"/>
-      <c r="H338" s="68"/>
-      <c r="I338" s="64"/>
-      <c r="J338" s="64"/>
-      <c r="K338" s="64"/>
-      <c r="L338" s="64"/>
-      <c r="M338" s="64"/>
-      <c r="N338" s="64"/>
-      <c r="O338" s="64"/>
-      <c r="P338" s="66"/>
+      <c r="B338" s="59"/>
+      <c r="C338" s="60"/>
+      <c r="D338" s="60"/>
+      <c r="E338" s="60"/>
+      <c r="F338" s="60"/>
+      <c r="G338" s="62"/>
+      <c r="H338" s="64"/>
+      <c r="I338" s="60"/>
+      <c r="J338" s="60"/>
+      <c r="K338" s="60"/>
+      <c r="L338" s="60"/>
+      <c r="M338" s="60"/>
+      <c r="N338" s="60"/>
+      <c r="O338" s="60"/>
+      <c r="P338" s="62"/>
     </row>
     <row r="339" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B339" s="5"/>
@@ -7403,46 +7401,46 @@
       <c r="P354" s="20"/>
     </row>
     <row r="355" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B355" s="61" t="s">
+      <c r="B355" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C355" s="62"/>
-      <c r="D355" s="62" t="s">
+      <c r="C355" s="58"/>
+      <c r="D355" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E355" s="62"/>
-      <c r="F355" s="62"/>
-      <c r="G355" s="65"/>
-      <c r="H355" s="67" t="s">
+      <c r="E355" s="58"/>
+      <c r="F355" s="58"/>
+      <c r="G355" s="61"/>
+      <c r="H355" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I355" s="62" t="s">
+      <c r="I355" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J355" s="62"/>
-      <c r="K355" s="62"/>
-      <c r="L355" s="62"/>
-      <c r="M355" s="62"/>
-      <c r="N355" s="62"/>
-      <c r="O355" s="62"/>
-      <c r="P355" s="65"/>
+      <c r="J355" s="58"/>
+      <c r="K355" s="58"/>
+      <c r="L355" s="58"/>
+      <c r="M355" s="58"/>
+      <c r="N355" s="58"/>
+      <c r="O355" s="58"/>
+      <c r="P355" s="61"/>
     </row>
     <row r="356" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B356" s="63"/>
-      <c r="C356" s="64"/>
-      <c r="D356" s="64"/>
-      <c r="E356" s="64"/>
-      <c r="F356" s="64"/>
-      <c r="G356" s="66"/>
-      <c r="H356" s="68"/>
-      <c r="I356" s="64"/>
-      <c r="J356" s="64"/>
-      <c r="K356" s="64"/>
-      <c r="L356" s="64"/>
-      <c r="M356" s="64"/>
-      <c r="N356" s="64"/>
-      <c r="O356" s="64"/>
-      <c r="P356" s="66"/>
+      <c r="B356" s="59"/>
+      <c r="C356" s="60"/>
+      <c r="D356" s="60"/>
+      <c r="E356" s="60"/>
+      <c r="F356" s="60"/>
+      <c r="G356" s="62"/>
+      <c r="H356" s="64"/>
+      <c r="I356" s="60"/>
+      <c r="J356" s="60"/>
+      <c r="K356" s="60"/>
+      <c r="L356" s="60"/>
+      <c r="M356" s="60"/>
+      <c r="N356" s="60"/>
+      <c r="O356" s="60"/>
+      <c r="P356" s="62"/>
     </row>
     <row r="357" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B357" s="5"/>
@@ -7692,46 +7690,46 @@
       <c r="P372" s="20"/>
     </row>
     <row r="373" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B373" s="61" t="s">
+      <c r="B373" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C373" s="62"/>
-      <c r="D373" s="62" t="s">
+      <c r="C373" s="58"/>
+      <c r="D373" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E373" s="62"/>
-      <c r="F373" s="62"/>
-      <c r="G373" s="65"/>
-      <c r="H373" s="67" t="s">
+      <c r="E373" s="58"/>
+      <c r="F373" s="58"/>
+      <c r="G373" s="61"/>
+      <c r="H373" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I373" s="62" t="s">
+      <c r="I373" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J373" s="62"/>
-      <c r="K373" s="62"/>
-      <c r="L373" s="62"/>
-      <c r="M373" s="62"/>
-      <c r="N373" s="62"/>
-      <c r="O373" s="62"/>
-      <c r="P373" s="65"/>
+      <c r="J373" s="58"/>
+      <c r="K373" s="58"/>
+      <c r="L373" s="58"/>
+      <c r="M373" s="58"/>
+      <c r="N373" s="58"/>
+      <c r="O373" s="58"/>
+      <c r="P373" s="61"/>
     </row>
     <row r="374" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B374" s="63"/>
-      <c r="C374" s="64"/>
-      <c r="D374" s="64"/>
-      <c r="E374" s="64"/>
-      <c r="F374" s="64"/>
-      <c r="G374" s="66"/>
-      <c r="H374" s="68"/>
-      <c r="I374" s="64"/>
-      <c r="J374" s="64"/>
-      <c r="K374" s="64"/>
-      <c r="L374" s="64"/>
-      <c r="M374" s="64"/>
-      <c r="N374" s="64"/>
-      <c r="O374" s="64"/>
-      <c r="P374" s="66"/>
+      <c r="B374" s="59"/>
+      <c r="C374" s="60"/>
+      <c r="D374" s="60"/>
+      <c r="E374" s="60"/>
+      <c r="F374" s="60"/>
+      <c r="G374" s="62"/>
+      <c r="H374" s="64"/>
+      <c r="I374" s="60"/>
+      <c r="J374" s="60"/>
+      <c r="K374" s="60"/>
+      <c r="L374" s="60"/>
+      <c r="M374" s="60"/>
+      <c r="N374" s="60"/>
+      <c r="O374" s="60"/>
+      <c r="P374" s="62"/>
     </row>
     <row r="375" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B375" s="5"/>
@@ -7981,46 +7979,46 @@
       <c r="P390" s="20"/>
     </row>
     <row r="391" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B391" s="61" t="s">
+      <c r="B391" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C391" s="62"/>
-      <c r="D391" s="62" t="s">
+      <c r="C391" s="58"/>
+      <c r="D391" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E391" s="62"/>
-      <c r="F391" s="62"/>
-      <c r="G391" s="65"/>
-      <c r="H391" s="67" t="s">
+      <c r="E391" s="58"/>
+      <c r="F391" s="58"/>
+      <c r="G391" s="61"/>
+      <c r="H391" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I391" s="62" t="s">
+      <c r="I391" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J391" s="62"/>
-      <c r="K391" s="62"/>
-      <c r="L391" s="62"/>
-      <c r="M391" s="62"/>
-      <c r="N391" s="62"/>
-      <c r="O391" s="62"/>
-      <c r="P391" s="65"/>
+      <c r="J391" s="58"/>
+      <c r="K391" s="58"/>
+      <c r="L391" s="58"/>
+      <c r="M391" s="58"/>
+      <c r="N391" s="58"/>
+      <c r="O391" s="58"/>
+      <c r="P391" s="61"/>
     </row>
     <row r="392" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B392" s="63"/>
-      <c r="C392" s="64"/>
-      <c r="D392" s="64"/>
-      <c r="E392" s="64"/>
-      <c r="F392" s="64"/>
-      <c r="G392" s="66"/>
-      <c r="H392" s="68"/>
-      <c r="I392" s="64"/>
-      <c r="J392" s="64"/>
-      <c r="K392" s="64"/>
-      <c r="L392" s="64"/>
-      <c r="M392" s="64"/>
-      <c r="N392" s="64"/>
-      <c r="O392" s="64"/>
-      <c r="P392" s="66"/>
+      <c r="B392" s="59"/>
+      <c r="C392" s="60"/>
+      <c r="D392" s="60"/>
+      <c r="E392" s="60"/>
+      <c r="F392" s="60"/>
+      <c r="G392" s="62"/>
+      <c r="H392" s="64"/>
+      <c r="I392" s="60"/>
+      <c r="J392" s="60"/>
+      <c r="K392" s="60"/>
+      <c r="L392" s="60"/>
+      <c r="M392" s="60"/>
+      <c r="N392" s="60"/>
+      <c r="O392" s="60"/>
+      <c r="P392" s="62"/>
     </row>
     <row r="393" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B393" s="5"/>
@@ -8270,46 +8268,46 @@
       <c r="P408" s="20"/>
     </row>
     <row r="409" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B409" s="61" t="s">
+      <c r="B409" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C409" s="62"/>
-      <c r="D409" s="62" t="s">
+      <c r="C409" s="58"/>
+      <c r="D409" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E409" s="62"/>
-      <c r="F409" s="62"/>
-      <c r="G409" s="65"/>
-      <c r="H409" s="67" t="s">
+      <c r="E409" s="58"/>
+      <c r="F409" s="58"/>
+      <c r="G409" s="61"/>
+      <c r="H409" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I409" s="62" t="s">
+      <c r="I409" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J409" s="62"/>
-      <c r="K409" s="62"/>
-      <c r="L409" s="62"/>
-      <c r="M409" s="62"/>
-      <c r="N409" s="62"/>
-      <c r="O409" s="62"/>
-      <c r="P409" s="65"/>
+      <c r="J409" s="58"/>
+      <c r="K409" s="58"/>
+      <c r="L409" s="58"/>
+      <c r="M409" s="58"/>
+      <c r="N409" s="58"/>
+      <c r="O409" s="58"/>
+      <c r="P409" s="61"/>
     </row>
     <row r="410" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B410" s="63"/>
-      <c r="C410" s="64"/>
-      <c r="D410" s="64"/>
-      <c r="E410" s="64"/>
-      <c r="F410" s="64"/>
-      <c r="G410" s="66"/>
-      <c r="H410" s="68"/>
-      <c r="I410" s="64"/>
-      <c r="J410" s="64"/>
-      <c r="K410" s="64"/>
-      <c r="L410" s="64"/>
-      <c r="M410" s="64"/>
-      <c r="N410" s="64"/>
-      <c r="O410" s="64"/>
-      <c r="P410" s="66"/>
+      <c r="B410" s="59"/>
+      <c r="C410" s="60"/>
+      <c r="D410" s="60"/>
+      <c r="E410" s="60"/>
+      <c r="F410" s="60"/>
+      <c r="G410" s="62"/>
+      <c r="H410" s="64"/>
+      <c r="I410" s="60"/>
+      <c r="J410" s="60"/>
+      <c r="K410" s="60"/>
+      <c r="L410" s="60"/>
+      <c r="M410" s="60"/>
+      <c r="N410" s="60"/>
+      <c r="O410" s="60"/>
+      <c r="P410" s="62"/>
     </row>
     <row r="411" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B411" s="5"/>
@@ -8559,46 +8557,46 @@
       <c r="P426" s="20"/>
     </row>
     <row r="427" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B427" s="61" t="s">
+      <c r="B427" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C427" s="62"/>
-      <c r="D427" s="62" t="s">
+      <c r="C427" s="58"/>
+      <c r="D427" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E427" s="62"/>
-      <c r="F427" s="62"/>
-      <c r="G427" s="65"/>
-      <c r="H427" s="67" t="s">
+      <c r="E427" s="58"/>
+      <c r="F427" s="58"/>
+      <c r="G427" s="61"/>
+      <c r="H427" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I427" s="62" t="s">
+      <c r="I427" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J427" s="62"/>
-      <c r="K427" s="62"/>
-      <c r="L427" s="62"/>
-      <c r="M427" s="62"/>
-      <c r="N427" s="62"/>
-      <c r="O427" s="62"/>
-      <c r="P427" s="65"/>
+      <c r="J427" s="58"/>
+      <c r="K427" s="58"/>
+      <c r="L427" s="58"/>
+      <c r="M427" s="58"/>
+      <c r="N427" s="58"/>
+      <c r="O427" s="58"/>
+      <c r="P427" s="61"/>
     </row>
     <row r="428" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B428" s="63"/>
-      <c r="C428" s="64"/>
-      <c r="D428" s="64"/>
-      <c r="E428" s="64"/>
-      <c r="F428" s="64"/>
-      <c r="G428" s="66"/>
-      <c r="H428" s="68"/>
-      <c r="I428" s="64"/>
-      <c r="J428" s="64"/>
-      <c r="K428" s="64"/>
-      <c r="L428" s="64"/>
-      <c r="M428" s="64"/>
-      <c r="N428" s="64"/>
-      <c r="O428" s="64"/>
-      <c r="P428" s="66"/>
+      <c r="B428" s="59"/>
+      <c r="C428" s="60"/>
+      <c r="D428" s="60"/>
+      <c r="E428" s="60"/>
+      <c r="F428" s="60"/>
+      <c r="G428" s="62"/>
+      <c r="H428" s="64"/>
+      <c r="I428" s="60"/>
+      <c r="J428" s="60"/>
+      <c r="K428" s="60"/>
+      <c r="L428" s="60"/>
+      <c r="M428" s="60"/>
+      <c r="N428" s="60"/>
+      <c r="O428" s="60"/>
+      <c r="P428" s="62"/>
     </row>
     <row r="429" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B429" s="5"/>
@@ -8848,46 +8846,46 @@
       <c r="P444" s="20"/>
     </row>
     <row r="445" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B445" s="61" t="s">
+      <c r="B445" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C445" s="62"/>
-      <c r="D445" s="62" t="s">
+      <c r="C445" s="58"/>
+      <c r="D445" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E445" s="62"/>
-      <c r="F445" s="62"/>
-      <c r="G445" s="65"/>
-      <c r="H445" s="67" t="s">
+      <c r="E445" s="58"/>
+      <c r="F445" s="58"/>
+      <c r="G445" s="61"/>
+      <c r="H445" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I445" s="62" t="s">
+      <c r="I445" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J445" s="62"/>
-      <c r="K445" s="62"/>
-      <c r="L445" s="62"/>
-      <c r="M445" s="62"/>
-      <c r="N445" s="62"/>
-      <c r="O445" s="62"/>
-      <c r="P445" s="65"/>
+      <c r="J445" s="58"/>
+      <c r="K445" s="58"/>
+      <c r="L445" s="58"/>
+      <c r="M445" s="58"/>
+      <c r="N445" s="58"/>
+      <c r="O445" s="58"/>
+      <c r="P445" s="61"/>
     </row>
     <row r="446" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B446" s="63"/>
-      <c r="C446" s="64"/>
-      <c r="D446" s="64"/>
-      <c r="E446" s="64"/>
-      <c r="F446" s="64"/>
-      <c r="G446" s="66"/>
-      <c r="H446" s="68"/>
-      <c r="I446" s="64"/>
-      <c r="J446" s="64"/>
-      <c r="K446" s="64"/>
-      <c r="L446" s="64"/>
-      <c r="M446" s="64"/>
-      <c r="N446" s="64"/>
-      <c r="O446" s="64"/>
-      <c r="P446" s="66"/>
+      <c r="B446" s="59"/>
+      <c r="C446" s="60"/>
+      <c r="D446" s="60"/>
+      <c r="E446" s="60"/>
+      <c r="F446" s="60"/>
+      <c r="G446" s="62"/>
+      <c r="H446" s="64"/>
+      <c r="I446" s="60"/>
+      <c r="J446" s="60"/>
+      <c r="K446" s="60"/>
+      <c r="L446" s="60"/>
+      <c r="M446" s="60"/>
+      <c r="N446" s="60"/>
+      <c r="O446" s="60"/>
+      <c r="P446" s="62"/>
     </row>
     <row r="447" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B447" s="5"/>
@@ -9137,46 +9135,46 @@
       <c r="P462" s="20"/>
     </row>
     <row r="463" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B463" s="61" t="s">
+      <c r="B463" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C463" s="62"/>
-      <c r="D463" s="62" t="s">
+      <c r="C463" s="58"/>
+      <c r="D463" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E463" s="62"/>
-      <c r="F463" s="62"/>
-      <c r="G463" s="65"/>
-      <c r="H463" s="67" t="s">
+      <c r="E463" s="58"/>
+      <c r="F463" s="58"/>
+      <c r="G463" s="61"/>
+      <c r="H463" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I463" s="62" t="s">
+      <c r="I463" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J463" s="62"/>
-      <c r="K463" s="62"/>
-      <c r="L463" s="62"/>
-      <c r="M463" s="62"/>
-      <c r="N463" s="62"/>
-      <c r="O463" s="62"/>
-      <c r="P463" s="65"/>
+      <c r="J463" s="58"/>
+      <c r="K463" s="58"/>
+      <c r="L463" s="58"/>
+      <c r="M463" s="58"/>
+      <c r="N463" s="58"/>
+      <c r="O463" s="58"/>
+      <c r="P463" s="61"/>
     </row>
     <row r="464" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B464" s="63"/>
-      <c r="C464" s="64"/>
-      <c r="D464" s="64"/>
-      <c r="E464" s="64"/>
-      <c r="F464" s="64"/>
-      <c r="G464" s="66"/>
-      <c r="H464" s="68"/>
-      <c r="I464" s="64"/>
-      <c r="J464" s="64"/>
-      <c r="K464" s="64"/>
-      <c r="L464" s="64"/>
-      <c r="M464" s="64"/>
-      <c r="N464" s="64"/>
-      <c r="O464" s="64"/>
-      <c r="P464" s="66"/>
+      <c r="B464" s="59"/>
+      <c r="C464" s="60"/>
+      <c r="D464" s="60"/>
+      <c r="E464" s="60"/>
+      <c r="F464" s="60"/>
+      <c r="G464" s="62"/>
+      <c r="H464" s="64"/>
+      <c r="I464" s="60"/>
+      <c r="J464" s="60"/>
+      <c r="K464" s="60"/>
+      <c r="L464" s="60"/>
+      <c r="M464" s="60"/>
+      <c r="N464" s="60"/>
+      <c r="O464" s="60"/>
+      <c r="P464" s="62"/>
     </row>
     <row r="465" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B465" s="5"/>
@@ -9426,46 +9424,46 @@
       <c r="P480" s="20"/>
     </row>
     <row r="481" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B481" s="61" t="s">
+      <c r="B481" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C481" s="62"/>
-      <c r="D481" s="62" t="s">
+      <c r="C481" s="58"/>
+      <c r="D481" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E481" s="62"/>
-      <c r="F481" s="62"/>
-      <c r="G481" s="65"/>
-      <c r="H481" s="67" t="s">
+      <c r="E481" s="58"/>
+      <c r="F481" s="58"/>
+      <c r="G481" s="61"/>
+      <c r="H481" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I481" s="62" t="s">
+      <c r="I481" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J481" s="62"/>
-      <c r="K481" s="62"/>
-      <c r="L481" s="62"/>
-      <c r="M481" s="62"/>
-      <c r="N481" s="62"/>
-      <c r="O481" s="62"/>
-      <c r="P481" s="65"/>
+      <c r="J481" s="58"/>
+      <c r="K481" s="58"/>
+      <c r="L481" s="58"/>
+      <c r="M481" s="58"/>
+      <c r="N481" s="58"/>
+      <c r="O481" s="58"/>
+      <c r="P481" s="61"/>
     </row>
     <row r="482" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B482" s="63"/>
-      <c r="C482" s="64"/>
-      <c r="D482" s="64"/>
-      <c r="E482" s="64"/>
-      <c r="F482" s="64"/>
-      <c r="G482" s="66"/>
-      <c r="H482" s="68"/>
-      <c r="I482" s="64"/>
-      <c r="J482" s="64"/>
-      <c r="K482" s="64"/>
-      <c r="L482" s="64"/>
-      <c r="M482" s="64"/>
-      <c r="N482" s="64"/>
-      <c r="O482" s="64"/>
-      <c r="P482" s="66"/>
+      <c r="B482" s="59"/>
+      <c r="C482" s="60"/>
+      <c r="D482" s="60"/>
+      <c r="E482" s="60"/>
+      <c r="F482" s="60"/>
+      <c r="G482" s="62"/>
+      <c r="H482" s="64"/>
+      <c r="I482" s="60"/>
+      <c r="J482" s="60"/>
+      <c r="K482" s="60"/>
+      <c r="L482" s="60"/>
+      <c r="M482" s="60"/>
+      <c r="N482" s="60"/>
+      <c r="O482" s="60"/>
+      <c r="P482" s="62"/>
     </row>
     <row r="483" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B483" s="5"/>
@@ -9715,46 +9713,46 @@
       <c r="P498" s="20"/>
     </row>
     <row r="499" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B499" s="61" t="s">
+      <c r="B499" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C499" s="62"/>
-      <c r="D499" s="62" t="s">
+      <c r="C499" s="58"/>
+      <c r="D499" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E499" s="62"/>
-      <c r="F499" s="62"/>
-      <c r="G499" s="65"/>
-      <c r="H499" s="67" t="s">
+      <c r="E499" s="58"/>
+      <c r="F499" s="58"/>
+      <c r="G499" s="61"/>
+      <c r="H499" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I499" s="62" t="s">
+      <c r="I499" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J499" s="62"/>
-      <c r="K499" s="62"/>
-      <c r="L499" s="62"/>
-      <c r="M499" s="62"/>
-      <c r="N499" s="62"/>
-      <c r="O499" s="62"/>
-      <c r="P499" s="65"/>
+      <c r="J499" s="58"/>
+      <c r="K499" s="58"/>
+      <c r="L499" s="58"/>
+      <c r="M499" s="58"/>
+      <c r="N499" s="58"/>
+      <c r="O499" s="58"/>
+      <c r="P499" s="61"/>
     </row>
     <row r="500" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B500" s="63"/>
-      <c r="C500" s="64"/>
-      <c r="D500" s="64"/>
-      <c r="E500" s="64"/>
-      <c r="F500" s="64"/>
-      <c r="G500" s="66"/>
-      <c r="H500" s="68"/>
-      <c r="I500" s="64"/>
-      <c r="J500" s="64"/>
-      <c r="K500" s="64"/>
-      <c r="L500" s="64"/>
-      <c r="M500" s="64"/>
-      <c r="N500" s="64"/>
-      <c r="O500" s="64"/>
-      <c r="P500" s="66"/>
+      <c r="B500" s="59"/>
+      <c r="C500" s="60"/>
+      <c r="D500" s="60"/>
+      <c r="E500" s="60"/>
+      <c r="F500" s="60"/>
+      <c r="G500" s="62"/>
+      <c r="H500" s="64"/>
+      <c r="I500" s="60"/>
+      <c r="J500" s="60"/>
+      <c r="K500" s="60"/>
+      <c r="L500" s="60"/>
+      <c r="M500" s="60"/>
+      <c r="N500" s="60"/>
+      <c r="O500" s="60"/>
+      <c r="P500" s="62"/>
     </row>
     <row r="501" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B501" s="5"/>
@@ -10004,46 +10002,46 @@
       <c r="P516" s="20"/>
     </row>
     <row r="517" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B517" s="61" t="s">
+      <c r="B517" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C517" s="62"/>
-      <c r="D517" s="62" t="s">
+      <c r="C517" s="58"/>
+      <c r="D517" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E517" s="62"/>
-      <c r="F517" s="62"/>
-      <c r="G517" s="65"/>
-      <c r="H517" s="67" t="s">
+      <c r="E517" s="58"/>
+      <c r="F517" s="58"/>
+      <c r="G517" s="61"/>
+      <c r="H517" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I517" s="62" t="s">
+      <c r="I517" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J517" s="62"/>
-      <c r="K517" s="62"/>
-      <c r="L517" s="62"/>
-      <c r="M517" s="62"/>
-      <c r="N517" s="62"/>
-      <c r="O517" s="62"/>
-      <c r="P517" s="65"/>
+      <c r="J517" s="58"/>
+      <c r="K517" s="58"/>
+      <c r="L517" s="58"/>
+      <c r="M517" s="58"/>
+      <c r="N517" s="58"/>
+      <c r="O517" s="58"/>
+      <c r="P517" s="61"/>
     </row>
     <row r="518" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B518" s="63"/>
-      <c r="C518" s="64"/>
-      <c r="D518" s="64"/>
-      <c r="E518" s="64"/>
-      <c r="F518" s="64"/>
-      <c r="G518" s="66"/>
-      <c r="H518" s="68"/>
-      <c r="I518" s="64"/>
-      <c r="J518" s="64"/>
-      <c r="K518" s="64"/>
-      <c r="L518" s="64"/>
-      <c r="M518" s="64"/>
-      <c r="N518" s="64"/>
-      <c r="O518" s="64"/>
-      <c r="P518" s="66"/>
+      <c r="B518" s="59"/>
+      <c r="C518" s="60"/>
+      <c r="D518" s="60"/>
+      <c r="E518" s="60"/>
+      <c r="F518" s="60"/>
+      <c r="G518" s="62"/>
+      <c r="H518" s="64"/>
+      <c r="I518" s="60"/>
+      <c r="J518" s="60"/>
+      <c r="K518" s="60"/>
+      <c r="L518" s="60"/>
+      <c r="M518" s="60"/>
+      <c r="N518" s="60"/>
+      <c r="O518" s="60"/>
+      <c r="P518" s="62"/>
     </row>
     <row r="519" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B519" s="5"/>
@@ -10293,46 +10291,46 @@
       <c r="P534" s="20"/>
     </row>
     <row r="535" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B535" s="61" t="s">
+      <c r="B535" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C535" s="62"/>
-      <c r="D535" s="62" t="s">
+      <c r="C535" s="58"/>
+      <c r="D535" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E535" s="62"/>
-      <c r="F535" s="62"/>
-      <c r="G535" s="65"/>
-      <c r="H535" s="67" t="s">
+      <c r="E535" s="58"/>
+      <c r="F535" s="58"/>
+      <c r="G535" s="61"/>
+      <c r="H535" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I535" s="62" t="s">
+      <c r="I535" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J535" s="62"/>
-      <c r="K535" s="62"/>
-      <c r="L535" s="62"/>
-      <c r="M535" s="62"/>
-      <c r="N535" s="62"/>
-      <c r="O535" s="62"/>
-      <c r="P535" s="65"/>
+      <c r="J535" s="58"/>
+      <c r="K535" s="58"/>
+      <c r="L535" s="58"/>
+      <c r="M535" s="58"/>
+      <c r="N535" s="58"/>
+      <c r="O535" s="58"/>
+      <c r="P535" s="61"/>
     </row>
     <row r="536" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B536" s="63"/>
-      <c r="C536" s="64"/>
-      <c r="D536" s="64"/>
-      <c r="E536" s="64"/>
-      <c r="F536" s="64"/>
-      <c r="G536" s="66"/>
-      <c r="H536" s="68"/>
-      <c r="I536" s="64"/>
-      <c r="J536" s="64"/>
-      <c r="K536" s="64"/>
-      <c r="L536" s="64"/>
-      <c r="M536" s="64"/>
-      <c r="N536" s="64"/>
-      <c r="O536" s="64"/>
-      <c r="P536" s="66"/>
+      <c r="B536" s="59"/>
+      <c r="C536" s="60"/>
+      <c r="D536" s="60"/>
+      <c r="E536" s="60"/>
+      <c r="F536" s="60"/>
+      <c r="G536" s="62"/>
+      <c r="H536" s="64"/>
+      <c r="I536" s="60"/>
+      <c r="J536" s="60"/>
+      <c r="K536" s="60"/>
+      <c r="L536" s="60"/>
+      <c r="M536" s="60"/>
+      <c r="N536" s="60"/>
+      <c r="O536" s="60"/>
+      <c r="P536" s="62"/>
     </row>
     <row r="537" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B537" s="5"/>
@@ -10582,46 +10580,46 @@
       <c r="P552" s="20"/>
     </row>
     <row r="553" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B553" s="61" t="s">
+      <c r="B553" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C553" s="62"/>
-      <c r="D553" s="62" t="s">
+      <c r="C553" s="58"/>
+      <c r="D553" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E553" s="62"/>
-      <c r="F553" s="62"/>
-      <c r="G553" s="65"/>
-      <c r="H553" s="67" t="s">
+      <c r="E553" s="58"/>
+      <c r="F553" s="58"/>
+      <c r="G553" s="61"/>
+      <c r="H553" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I553" s="62" t="s">
+      <c r="I553" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J553" s="62"/>
-      <c r="K553" s="62"/>
-      <c r="L553" s="62"/>
-      <c r="M553" s="62"/>
-      <c r="N553" s="62"/>
-      <c r="O553" s="62"/>
-      <c r="P553" s="65"/>
+      <c r="J553" s="58"/>
+      <c r="K553" s="58"/>
+      <c r="L553" s="58"/>
+      <c r="M553" s="58"/>
+      <c r="N553" s="58"/>
+      <c r="O553" s="58"/>
+      <c r="P553" s="61"/>
     </row>
     <row r="554" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B554" s="63"/>
-      <c r="C554" s="64"/>
-      <c r="D554" s="64"/>
-      <c r="E554" s="64"/>
-      <c r="F554" s="64"/>
-      <c r="G554" s="66"/>
-      <c r="H554" s="68"/>
-      <c r="I554" s="64"/>
-      <c r="J554" s="64"/>
-      <c r="K554" s="64"/>
-      <c r="L554" s="64"/>
-      <c r="M554" s="64"/>
-      <c r="N554" s="64"/>
-      <c r="O554" s="64"/>
-      <c r="P554" s="66"/>
+      <c r="B554" s="59"/>
+      <c r="C554" s="60"/>
+      <c r="D554" s="60"/>
+      <c r="E554" s="60"/>
+      <c r="F554" s="60"/>
+      <c r="G554" s="62"/>
+      <c r="H554" s="64"/>
+      <c r="I554" s="60"/>
+      <c r="J554" s="60"/>
+      <c r="K554" s="60"/>
+      <c r="L554" s="60"/>
+      <c r="M554" s="60"/>
+      <c r="N554" s="60"/>
+      <c r="O554" s="60"/>
+      <c r="P554" s="62"/>
     </row>
     <row r="555" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B555" s="5"/>
@@ -10871,46 +10869,46 @@
       <c r="P570" s="20"/>
     </row>
     <row r="571" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B571" s="61" t="s">
+      <c r="B571" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C571" s="62"/>
-      <c r="D571" s="62" t="s">
+      <c r="C571" s="58"/>
+      <c r="D571" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E571" s="62"/>
-      <c r="F571" s="62"/>
-      <c r="G571" s="65"/>
-      <c r="H571" s="67" t="s">
+      <c r="E571" s="58"/>
+      <c r="F571" s="58"/>
+      <c r="G571" s="61"/>
+      <c r="H571" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I571" s="62" t="s">
+      <c r="I571" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J571" s="62"/>
-      <c r="K571" s="62"/>
-      <c r="L571" s="62"/>
-      <c r="M571" s="62"/>
-      <c r="N571" s="62"/>
-      <c r="O571" s="62"/>
-      <c r="P571" s="65"/>
+      <c r="J571" s="58"/>
+      <c r="K571" s="58"/>
+      <c r="L571" s="58"/>
+      <c r="M571" s="58"/>
+      <c r="N571" s="58"/>
+      <c r="O571" s="58"/>
+      <c r="P571" s="61"/>
     </row>
     <row r="572" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B572" s="63"/>
-      <c r="C572" s="64"/>
-      <c r="D572" s="64"/>
-      <c r="E572" s="64"/>
-      <c r="F572" s="64"/>
-      <c r="G572" s="66"/>
-      <c r="H572" s="68"/>
-      <c r="I572" s="64"/>
-      <c r="J572" s="64"/>
-      <c r="K572" s="64"/>
-      <c r="L572" s="64"/>
-      <c r="M572" s="64"/>
-      <c r="N572" s="64"/>
-      <c r="O572" s="64"/>
-      <c r="P572" s="66"/>
+      <c r="B572" s="59"/>
+      <c r="C572" s="60"/>
+      <c r="D572" s="60"/>
+      <c r="E572" s="60"/>
+      <c r="F572" s="60"/>
+      <c r="G572" s="62"/>
+      <c r="H572" s="64"/>
+      <c r="I572" s="60"/>
+      <c r="J572" s="60"/>
+      <c r="K572" s="60"/>
+      <c r="L572" s="60"/>
+      <c r="M572" s="60"/>
+      <c r="N572" s="60"/>
+      <c r="O572" s="60"/>
+      <c r="P572" s="62"/>
     </row>
     <row r="573" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B573" s="5"/>
@@ -11160,46 +11158,46 @@
       <c r="P588" s="20"/>
     </row>
     <row r="589" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B589" s="61" t="s">
+      <c r="B589" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C589" s="62"/>
-      <c r="D589" s="62" t="s">
+      <c r="C589" s="58"/>
+      <c r="D589" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E589" s="62"/>
-      <c r="F589" s="62"/>
-      <c r="G589" s="65"/>
-      <c r="H589" s="67" t="s">
+      <c r="E589" s="58"/>
+      <c r="F589" s="58"/>
+      <c r="G589" s="61"/>
+      <c r="H589" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I589" s="62" t="s">
+      <c r="I589" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J589" s="62"/>
-      <c r="K589" s="62"/>
-      <c r="L589" s="62"/>
-      <c r="M589" s="62"/>
-      <c r="N589" s="62"/>
-      <c r="O589" s="62"/>
-      <c r="P589" s="65"/>
+      <c r="J589" s="58"/>
+      <c r="K589" s="58"/>
+      <c r="L589" s="58"/>
+      <c r="M589" s="58"/>
+      <c r="N589" s="58"/>
+      <c r="O589" s="58"/>
+      <c r="P589" s="61"/>
     </row>
     <row r="590" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B590" s="63"/>
-      <c r="C590" s="64"/>
-      <c r="D590" s="64"/>
-      <c r="E590" s="64"/>
-      <c r="F590" s="64"/>
-      <c r="G590" s="66"/>
-      <c r="H590" s="68"/>
-      <c r="I590" s="64"/>
-      <c r="J590" s="64"/>
-      <c r="K590" s="64"/>
-      <c r="L590" s="64"/>
-      <c r="M590" s="64"/>
-      <c r="N590" s="64"/>
-      <c r="O590" s="64"/>
-      <c r="P590" s="66"/>
+      <c r="B590" s="59"/>
+      <c r="C590" s="60"/>
+      <c r="D590" s="60"/>
+      <c r="E590" s="60"/>
+      <c r="F590" s="60"/>
+      <c r="G590" s="62"/>
+      <c r="H590" s="64"/>
+      <c r="I590" s="60"/>
+      <c r="J590" s="60"/>
+      <c r="K590" s="60"/>
+      <c r="L590" s="60"/>
+      <c r="M590" s="60"/>
+      <c r="N590" s="60"/>
+      <c r="O590" s="60"/>
+      <c r="P590" s="62"/>
     </row>
     <row r="591" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B591" s="5"/>
@@ -11449,46 +11447,46 @@
       <c r="P606" s="20"/>
     </row>
     <row r="607" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B607" s="61" t="s">
+      <c r="B607" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C607" s="62"/>
-      <c r="D607" s="62" t="s">
+      <c r="C607" s="58"/>
+      <c r="D607" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E607" s="62"/>
-      <c r="F607" s="62"/>
-      <c r="G607" s="65"/>
-      <c r="H607" s="67" t="s">
+      <c r="E607" s="58"/>
+      <c r="F607" s="58"/>
+      <c r="G607" s="61"/>
+      <c r="H607" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I607" s="62" t="s">
+      <c r="I607" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J607" s="62"/>
-      <c r="K607" s="62"/>
-      <c r="L607" s="62"/>
-      <c r="M607" s="62"/>
-      <c r="N607" s="62"/>
-      <c r="O607" s="62"/>
-      <c r="P607" s="65"/>
+      <c r="J607" s="58"/>
+      <c r="K607" s="58"/>
+      <c r="L607" s="58"/>
+      <c r="M607" s="58"/>
+      <c r="N607" s="58"/>
+      <c r="O607" s="58"/>
+      <c r="P607" s="61"/>
     </row>
     <row r="608" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B608" s="63"/>
-      <c r="C608" s="64"/>
-      <c r="D608" s="64"/>
-      <c r="E608" s="64"/>
-      <c r="F608" s="64"/>
-      <c r="G608" s="66"/>
-      <c r="H608" s="68"/>
-      <c r="I608" s="64"/>
-      <c r="J608" s="64"/>
-      <c r="K608" s="64"/>
-      <c r="L608" s="64"/>
-      <c r="M608" s="64"/>
-      <c r="N608" s="64"/>
-      <c r="O608" s="64"/>
-      <c r="P608" s="66"/>
+      <c r="B608" s="59"/>
+      <c r="C608" s="60"/>
+      <c r="D608" s="60"/>
+      <c r="E608" s="60"/>
+      <c r="F608" s="60"/>
+      <c r="G608" s="62"/>
+      <c r="H608" s="64"/>
+      <c r="I608" s="60"/>
+      <c r="J608" s="60"/>
+      <c r="K608" s="60"/>
+      <c r="L608" s="60"/>
+      <c r="M608" s="60"/>
+      <c r="N608" s="60"/>
+      <c r="O608" s="60"/>
+      <c r="P608" s="62"/>
     </row>
     <row r="609" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B609" s="5"/>
@@ -11738,46 +11736,46 @@
       <c r="P624" s="20"/>
     </row>
     <row r="625" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B625" s="61" t="s">
+      <c r="B625" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C625" s="62"/>
-      <c r="D625" s="62" t="s">
+      <c r="C625" s="58"/>
+      <c r="D625" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E625" s="62"/>
-      <c r="F625" s="62"/>
-      <c r="G625" s="65"/>
-      <c r="H625" s="67" t="s">
+      <c r="E625" s="58"/>
+      <c r="F625" s="58"/>
+      <c r="G625" s="61"/>
+      <c r="H625" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I625" s="62" t="s">
+      <c r="I625" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J625" s="62"/>
-      <c r="K625" s="62"/>
-      <c r="L625" s="62"/>
-      <c r="M625" s="62"/>
-      <c r="N625" s="62"/>
-      <c r="O625" s="62"/>
-      <c r="P625" s="65"/>
+      <c r="J625" s="58"/>
+      <c r="K625" s="58"/>
+      <c r="L625" s="58"/>
+      <c r="M625" s="58"/>
+      <c r="N625" s="58"/>
+      <c r="O625" s="58"/>
+      <c r="P625" s="61"/>
     </row>
     <row r="626" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B626" s="63"/>
-      <c r="C626" s="64"/>
-      <c r="D626" s="64"/>
-      <c r="E626" s="64"/>
-      <c r="F626" s="64"/>
-      <c r="G626" s="66"/>
-      <c r="H626" s="68"/>
-      <c r="I626" s="64"/>
-      <c r="J626" s="64"/>
-      <c r="K626" s="64"/>
-      <c r="L626" s="64"/>
-      <c r="M626" s="64"/>
-      <c r="N626" s="64"/>
-      <c r="O626" s="64"/>
-      <c r="P626" s="66"/>
+      <c r="B626" s="59"/>
+      <c r="C626" s="60"/>
+      <c r="D626" s="60"/>
+      <c r="E626" s="60"/>
+      <c r="F626" s="60"/>
+      <c r="G626" s="62"/>
+      <c r="H626" s="64"/>
+      <c r="I626" s="60"/>
+      <c r="J626" s="60"/>
+      <c r="K626" s="60"/>
+      <c r="L626" s="60"/>
+      <c r="M626" s="60"/>
+      <c r="N626" s="60"/>
+      <c r="O626" s="60"/>
+      <c r="P626" s="62"/>
     </row>
     <row r="627" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B627" s="5"/>
@@ -12027,46 +12025,46 @@
       <c r="P642" s="20"/>
     </row>
     <row r="643" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B643" s="61" t="s">
+      <c r="B643" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C643" s="62"/>
-      <c r="D643" s="62" t="s">
+      <c r="C643" s="58"/>
+      <c r="D643" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E643" s="62"/>
-      <c r="F643" s="62"/>
-      <c r="G643" s="65"/>
-      <c r="H643" s="67" t="s">
+      <c r="E643" s="58"/>
+      <c r="F643" s="58"/>
+      <c r="G643" s="61"/>
+      <c r="H643" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I643" s="62" t="s">
+      <c r="I643" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J643" s="62"/>
-      <c r="K643" s="62"/>
-      <c r="L643" s="62"/>
-      <c r="M643" s="62"/>
-      <c r="N643" s="62"/>
-      <c r="O643" s="62"/>
-      <c r="P643" s="65"/>
+      <c r="J643" s="58"/>
+      <c r="K643" s="58"/>
+      <c r="L643" s="58"/>
+      <c r="M643" s="58"/>
+      <c r="N643" s="58"/>
+      <c r="O643" s="58"/>
+      <c r="P643" s="61"/>
     </row>
     <row r="644" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B644" s="63"/>
-      <c r="C644" s="64"/>
-      <c r="D644" s="64"/>
-      <c r="E644" s="64"/>
-      <c r="F644" s="64"/>
-      <c r="G644" s="66"/>
-      <c r="H644" s="68"/>
-      <c r="I644" s="64"/>
-      <c r="J644" s="64"/>
-      <c r="K644" s="64"/>
-      <c r="L644" s="64"/>
-      <c r="M644" s="64"/>
-      <c r="N644" s="64"/>
-      <c r="O644" s="64"/>
-      <c r="P644" s="66"/>
+      <c r="B644" s="59"/>
+      <c r="C644" s="60"/>
+      <c r="D644" s="60"/>
+      <c r="E644" s="60"/>
+      <c r="F644" s="60"/>
+      <c r="G644" s="62"/>
+      <c r="H644" s="64"/>
+      <c r="I644" s="60"/>
+      <c r="J644" s="60"/>
+      <c r="K644" s="60"/>
+      <c r="L644" s="60"/>
+      <c r="M644" s="60"/>
+      <c r="N644" s="60"/>
+      <c r="O644" s="60"/>
+      <c r="P644" s="62"/>
     </row>
     <row r="645" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B645" s="5"/>
@@ -12316,46 +12314,46 @@
       <c r="P660" s="20"/>
     </row>
     <row r="661" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B661" s="61" t="s">
+      <c r="B661" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C661" s="62"/>
-      <c r="D661" s="62" t="s">
+      <c r="C661" s="58"/>
+      <c r="D661" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E661" s="62"/>
-      <c r="F661" s="62"/>
-      <c r="G661" s="65"/>
-      <c r="H661" s="67" t="s">
+      <c r="E661" s="58"/>
+      <c r="F661" s="58"/>
+      <c r="G661" s="61"/>
+      <c r="H661" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I661" s="62" t="s">
+      <c r="I661" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J661" s="62"/>
-      <c r="K661" s="62"/>
-      <c r="L661" s="62"/>
-      <c r="M661" s="62"/>
-      <c r="N661" s="62"/>
-      <c r="O661" s="62"/>
-      <c r="P661" s="65"/>
+      <c r="J661" s="58"/>
+      <c r="K661" s="58"/>
+      <c r="L661" s="58"/>
+      <c r="M661" s="58"/>
+      <c r="N661" s="58"/>
+      <c r="O661" s="58"/>
+      <c r="P661" s="61"/>
     </row>
     <row r="662" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B662" s="63"/>
-      <c r="C662" s="64"/>
-      <c r="D662" s="64"/>
-      <c r="E662" s="64"/>
-      <c r="F662" s="64"/>
-      <c r="G662" s="66"/>
-      <c r="H662" s="68"/>
-      <c r="I662" s="64"/>
-      <c r="J662" s="64"/>
-      <c r="K662" s="64"/>
-      <c r="L662" s="64"/>
-      <c r="M662" s="64"/>
-      <c r="N662" s="64"/>
-      <c r="O662" s="64"/>
-      <c r="P662" s="66"/>
+      <c r="B662" s="59"/>
+      <c r="C662" s="60"/>
+      <c r="D662" s="60"/>
+      <c r="E662" s="60"/>
+      <c r="F662" s="60"/>
+      <c r="G662" s="62"/>
+      <c r="H662" s="64"/>
+      <c r="I662" s="60"/>
+      <c r="J662" s="60"/>
+      <c r="K662" s="60"/>
+      <c r="L662" s="60"/>
+      <c r="M662" s="60"/>
+      <c r="N662" s="60"/>
+      <c r="O662" s="60"/>
+      <c r="P662" s="62"/>
     </row>
     <row r="663" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B663" s="5"/>
@@ -12605,46 +12603,46 @@
       <c r="P678" s="20"/>
     </row>
     <row r="679" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B679" s="61" t="s">
+      <c r="B679" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C679" s="62"/>
-      <c r="D679" s="62" t="s">
+      <c r="C679" s="58"/>
+      <c r="D679" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E679" s="62"/>
-      <c r="F679" s="62"/>
-      <c r="G679" s="65"/>
-      <c r="H679" s="67" t="s">
+      <c r="E679" s="58"/>
+      <c r="F679" s="58"/>
+      <c r="G679" s="61"/>
+      <c r="H679" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I679" s="62" t="s">
+      <c r="I679" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J679" s="62"/>
-      <c r="K679" s="62"/>
-      <c r="L679" s="62"/>
-      <c r="M679" s="62"/>
-      <c r="N679" s="62"/>
-      <c r="O679" s="62"/>
-      <c r="P679" s="65"/>
+      <c r="J679" s="58"/>
+      <c r="K679" s="58"/>
+      <c r="L679" s="58"/>
+      <c r="M679" s="58"/>
+      <c r="N679" s="58"/>
+      <c r="O679" s="58"/>
+      <c r="P679" s="61"/>
     </row>
     <row r="680" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B680" s="63"/>
-      <c r="C680" s="64"/>
-      <c r="D680" s="64"/>
-      <c r="E680" s="64"/>
-      <c r="F680" s="64"/>
-      <c r="G680" s="66"/>
-      <c r="H680" s="68"/>
-      <c r="I680" s="64"/>
-      <c r="J680" s="64"/>
-      <c r="K680" s="64"/>
-      <c r="L680" s="64"/>
-      <c r="M680" s="64"/>
-      <c r="N680" s="64"/>
-      <c r="O680" s="64"/>
-      <c r="P680" s="66"/>
+      <c r="B680" s="59"/>
+      <c r="C680" s="60"/>
+      <c r="D680" s="60"/>
+      <c r="E680" s="60"/>
+      <c r="F680" s="60"/>
+      <c r="G680" s="62"/>
+      <c r="H680" s="64"/>
+      <c r="I680" s="60"/>
+      <c r="J680" s="60"/>
+      <c r="K680" s="60"/>
+      <c r="L680" s="60"/>
+      <c r="M680" s="60"/>
+      <c r="N680" s="60"/>
+      <c r="O680" s="60"/>
+      <c r="P680" s="62"/>
     </row>
     <row r="681" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B681" s="5"/>
@@ -12894,46 +12892,46 @@
       <c r="P696" s="20"/>
     </row>
     <row r="697" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B697" s="61" t="s">
+      <c r="B697" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C697" s="62"/>
-      <c r="D697" s="62" t="s">
+      <c r="C697" s="58"/>
+      <c r="D697" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E697" s="62"/>
-      <c r="F697" s="62"/>
-      <c r="G697" s="65"/>
-      <c r="H697" s="67" t="s">
+      <c r="E697" s="58"/>
+      <c r="F697" s="58"/>
+      <c r="G697" s="61"/>
+      <c r="H697" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I697" s="62" t="s">
+      <c r="I697" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J697" s="62"/>
-      <c r="K697" s="62"/>
-      <c r="L697" s="62"/>
-      <c r="M697" s="62"/>
-      <c r="N697" s="62"/>
-      <c r="O697" s="62"/>
-      <c r="P697" s="65"/>
+      <c r="J697" s="58"/>
+      <c r="K697" s="58"/>
+      <c r="L697" s="58"/>
+      <c r="M697" s="58"/>
+      <c r="N697" s="58"/>
+      <c r="O697" s="58"/>
+      <c r="P697" s="61"/>
     </row>
     <row r="698" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B698" s="63"/>
-      <c r="C698" s="64"/>
-      <c r="D698" s="64"/>
-      <c r="E698" s="64"/>
-      <c r="F698" s="64"/>
-      <c r="G698" s="66"/>
-      <c r="H698" s="68"/>
-      <c r="I698" s="64"/>
-      <c r="J698" s="64"/>
-      <c r="K698" s="64"/>
-      <c r="L698" s="64"/>
-      <c r="M698" s="64"/>
-      <c r="N698" s="64"/>
-      <c r="O698" s="64"/>
-      <c r="P698" s="66"/>
+      <c r="B698" s="59"/>
+      <c r="C698" s="60"/>
+      <c r="D698" s="60"/>
+      <c r="E698" s="60"/>
+      <c r="F698" s="60"/>
+      <c r="G698" s="62"/>
+      <c r="H698" s="64"/>
+      <c r="I698" s="60"/>
+      <c r="J698" s="60"/>
+      <c r="K698" s="60"/>
+      <c r="L698" s="60"/>
+      <c r="M698" s="60"/>
+      <c r="N698" s="60"/>
+      <c r="O698" s="60"/>
+      <c r="P698" s="62"/>
     </row>
     <row r="699" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B699" s="5"/>
@@ -13183,46 +13181,46 @@
       <c r="P714" s="20"/>
     </row>
     <row r="715" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B715" s="61" t="s">
+      <c r="B715" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C715" s="62"/>
-      <c r="D715" s="62" t="s">
+      <c r="C715" s="58"/>
+      <c r="D715" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E715" s="62"/>
-      <c r="F715" s="62"/>
-      <c r="G715" s="65"/>
-      <c r="H715" s="67" t="s">
+      <c r="E715" s="58"/>
+      <c r="F715" s="58"/>
+      <c r="G715" s="61"/>
+      <c r="H715" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I715" s="62" t="s">
+      <c r="I715" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J715" s="62"/>
-      <c r="K715" s="62"/>
-      <c r="L715" s="62"/>
-      <c r="M715" s="62"/>
-      <c r="N715" s="62"/>
-      <c r="O715" s="62"/>
-      <c r="P715" s="65"/>
+      <c r="J715" s="58"/>
+      <c r="K715" s="58"/>
+      <c r="L715" s="58"/>
+      <c r="M715" s="58"/>
+      <c r="N715" s="58"/>
+      <c r="O715" s="58"/>
+      <c r="P715" s="61"/>
     </row>
     <row r="716" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B716" s="63"/>
-      <c r="C716" s="64"/>
-      <c r="D716" s="64"/>
-      <c r="E716" s="64"/>
-      <c r="F716" s="64"/>
-      <c r="G716" s="66"/>
-      <c r="H716" s="68"/>
-      <c r="I716" s="64"/>
-      <c r="J716" s="64"/>
-      <c r="K716" s="64"/>
-      <c r="L716" s="64"/>
-      <c r="M716" s="64"/>
-      <c r="N716" s="64"/>
-      <c r="O716" s="64"/>
-      <c r="P716" s="66"/>
+      <c r="B716" s="59"/>
+      <c r="C716" s="60"/>
+      <c r="D716" s="60"/>
+      <c r="E716" s="60"/>
+      <c r="F716" s="60"/>
+      <c r="G716" s="62"/>
+      <c r="H716" s="64"/>
+      <c r="I716" s="60"/>
+      <c r="J716" s="60"/>
+      <c r="K716" s="60"/>
+      <c r="L716" s="60"/>
+      <c r="M716" s="60"/>
+      <c r="N716" s="60"/>
+      <c r="O716" s="60"/>
+      <c r="P716" s="62"/>
     </row>
     <row r="717" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B717" s="5"/>
@@ -13472,46 +13470,46 @@
       <c r="P732" s="20"/>
     </row>
     <row r="733" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B733" s="61" t="s">
+      <c r="B733" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C733" s="62"/>
-      <c r="D733" s="62" t="s">
+      <c r="C733" s="58"/>
+      <c r="D733" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E733" s="62"/>
-      <c r="F733" s="62"/>
-      <c r="G733" s="65"/>
-      <c r="H733" s="67" t="s">
+      <c r="E733" s="58"/>
+      <c r="F733" s="58"/>
+      <c r="G733" s="61"/>
+      <c r="H733" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I733" s="62" t="s">
+      <c r="I733" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J733" s="62"/>
-      <c r="K733" s="62"/>
-      <c r="L733" s="62"/>
-      <c r="M733" s="62"/>
-      <c r="N733" s="62"/>
-      <c r="O733" s="62"/>
-      <c r="P733" s="65"/>
+      <c r="J733" s="58"/>
+      <c r="K733" s="58"/>
+      <c r="L733" s="58"/>
+      <c r="M733" s="58"/>
+      <c r="N733" s="58"/>
+      <c r="O733" s="58"/>
+      <c r="P733" s="61"/>
     </row>
     <row r="734" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B734" s="63"/>
-      <c r="C734" s="64"/>
-      <c r="D734" s="64"/>
-      <c r="E734" s="64"/>
-      <c r="F734" s="64"/>
-      <c r="G734" s="66"/>
-      <c r="H734" s="68"/>
-      <c r="I734" s="64"/>
-      <c r="J734" s="64"/>
-      <c r="K734" s="64"/>
-      <c r="L734" s="64"/>
-      <c r="M734" s="64"/>
-      <c r="N734" s="64"/>
-      <c r="O734" s="64"/>
-      <c r="P734" s="66"/>
+      <c r="B734" s="59"/>
+      <c r="C734" s="60"/>
+      <c r="D734" s="60"/>
+      <c r="E734" s="60"/>
+      <c r="F734" s="60"/>
+      <c r="G734" s="62"/>
+      <c r="H734" s="64"/>
+      <c r="I734" s="60"/>
+      <c r="J734" s="60"/>
+      <c r="K734" s="60"/>
+      <c r="L734" s="60"/>
+      <c r="M734" s="60"/>
+      <c r="N734" s="60"/>
+      <c r="O734" s="60"/>
+      <c r="P734" s="62"/>
     </row>
     <row r="735" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B735" s="5"/>
@@ -13761,46 +13759,46 @@
       <c r="P750" s="20"/>
     </row>
     <row r="751" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B751" s="61" t="s">
+      <c r="B751" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C751" s="62"/>
-      <c r="D751" s="62" t="s">
+      <c r="C751" s="58"/>
+      <c r="D751" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E751" s="62"/>
-      <c r="F751" s="62"/>
-      <c r="G751" s="65"/>
-      <c r="H751" s="67" t="s">
+      <c r="E751" s="58"/>
+      <c r="F751" s="58"/>
+      <c r="G751" s="61"/>
+      <c r="H751" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I751" s="62" t="s">
+      <c r="I751" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J751" s="62"/>
-      <c r="K751" s="62"/>
-      <c r="L751" s="62"/>
-      <c r="M751" s="62"/>
-      <c r="N751" s="62"/>
-      <c r="O751" s="62"/>
-      <c r="P751" s="65"/>
+      <c r="J751" s="58"/>
+      <c r="K751" s="58"/>
+      <c r="L751" s="58"/>
+      <c r="M751" s="58"/>
+      <c r="N751" s="58"/>
+      <c r="O751" s="58"/>
+      <c r="P751" s="61"/>
     </row>
     <row r="752" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B752" s="63"/>
-      <c r="C752" s="64"/>
-      <c r="D752" s="64"/>
-      <c r="E752" s="64"/>
-      <c r="F752" s="64"/>
-      <c r="G752" s="66"/>
-      <c r="H752" s="68"/>
-      <c r="I752" s="64"/>
-      <c r="J752" s="64"/>
-      <c r="K752" s="64"/>
-      <c r="L752" s="64"/>
-      <c r="M752" s="64"/>
-      <c r="N752" s="64"/>
-      <c r="O752" s="64"/>
-      <c r="P752" s="66"/>
+      <c r="B752" s="59"/>
+      <c r="C752" s="60"/>
+      <c r="D752" s="60"/>
+      <c r="E752" s="60"/>
+      <c r="F752" s="60"/>
+      <c r="G752" s="62"/>
+      <c r="H752" s="64"/>
+      <c r="I752" s="60"/>
+      <c r="J752" s="60"/>
+      <c r="K752" s="60"/>
+      <c r="L752" s="60"/>
+      <c r="M752" s="60"/>
+      <c r="N752" s="60"/>
+      <c r="O752" s="60"/>
+      <c r="P752" s="62"/>
     </row>
     <row r="753" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B753" s="5"/>
@@ -14050,46 +14048,46 @@
       <c r="P768" s="20"/>
     </row>
     <row r="769" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B769" s="61" t="s">
+      <c r="B769" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C769" s="62"/>
-      <c r="D769" s="62" t="s">
+      <c r="C769" s="58"/>
+      <c r="D769" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E769" s="62"/>
-      <c r="F769" s="62"/>
-      <c r="G769" s="65"/>
-      <c r="H769" s="67" t="s">
+      <c r="E769" s="58"/>
+      <c r="F769" s="58"/>
+      <c r="G769" s="61"/>
+      <c r="H769" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I769" s="62" t="s">
+      <c r="I769" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J769" s="62"/>
-      <c r="K769" s="62"/>
-      <c r="L769" s="62"/>
-      <c r="M769" s="62"/>
-      <c r="N769" s="62"/>
-      <c r="O769" s="62"/>
-      <c r="P769" s="65"/>
+      <c r="J769" s="58"/>
+      <c r="K769" s="58"/>
+      <c r="L769" s="58"/>
+      <c r="M769" s="58"/>
+      <c r="N769" s="58"/>
+      <c r="O769" s="58"/>
+      <c r="P769" s="61"/>
     </row>
     <row r="770" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B770" s="63"/>
-      <c r="C770" s="64"/>
-      <c r="D770" s="64"/>
-      <c r="E770" s="64"/>
-      <c r="F770" s="64"/>
-      <c r="G770" s="66"/>
-      <c r="H770" s="68"/>
-      <c r="I770" s="64"/>
-      <c r="J770" s="64"/>
-      <c r="K770" s="64"/>
-      <c r="L770" s="64"/>
-      <c r="M770" s="64"/>
-      <c r="N770" s="64"/>
-      <c r="O770" s="64"/>
-      <c r="P770" s="66"/>
+      <c r="B770" s="59"/>
+      <c r="C770" s="60"/>
+      <c r="D770" s="60"/>
+      <c r="E770" s="60"/>
+      <c r="F770" s="60"/>
+      <c r="G770" s="62"/>
+      <c r="H770" s="64"/>
+      <c r="I770" s="60"/>
+      <c r="J770" s="60"/>
+      <c r="K770" s="60"/>
+      <c r="L770" s="60"/>
+      <c r="M770" s="60"/>
+      <c r="N770" s="60"/>
+      <c r="O770" s="60"/>
+      <c r="P770" s="62"/>
     </row>
     <row r="771" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B771" s="5"/>
@@ -14339,46 +14337,46 @@
       <c r="P786" s="20"/>
     </row>
     <row r="787" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B787" s="61" t="s">
+      <c r="B787" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C787" s="62"/>
-      <c r="D787" s="62" t="s">
+      <c r="C787" s="58"/>
+      <c r="D787" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E787" s="62"/>
-      <c r="F787" s="62"/>
-      <c r="G787" s="65"/>
-      <c r="H787" s="67" t="s">
+      <c r="E787" s="58"/>
+      <c r="F787" s="58"/>
+      <c r="G787" s="61"/>
+      <c r="H787" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I787" s="62" t="s">
+      <c r="I787" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J787" s="62"/>
-      <c r="K787" s="62"/>
-      <c r="L787" s="62"/>
-      <c r="M787" s="62"/>
-      <c r="N787" s="62"/>
-      <c r="O787" s="62"/>
-      <c r="P787" s="65"/>
+      <c r="J787" s="58"/>
+      <c r="K787" s="58"/>
+      <c r="L787" s="58"/>
+      <c r="M787" s="58"/>
+      <c r="N787" s="58"/>
+      <c r="O787" s="58"/>
+      <c r="P787" s="61"/>
     </row>
     <row r="788" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B788" s="63"/>
-      <c r="C788" s="64"/>
-      <c r="D788" s="64"/>
-      <c r="E788" s="64"/>
-      <c r="F788" s="64"/>
-      <c r="G788" s="66"/>
-      <c r="H788" s="68"/>
-      <c r="I788" s="64"/>
-      <c r="J788" s="64"/>
-      <c r="K788" s="64"/>
-      <c r="L788" s="64"/>
-      <c r="M788" s="64"/>
-      <c r="N788" s="64"/>
-      <c r="O788" s="64"/>
-      <c r="P788" s="66"/>
+      <c r="B788" s="59"/>
+      <c r="C788" s="60"/>
+      <c r="D788" s="60"/>
+      <c r="E788" s="60"/>
+      <c r="F788" s="60"/>
+      <c r="G788" s="62"/>
+      <c r="H788" s="64"/>
+      <c r="I788" s="60"/>
+      <c r="J788" s="60"/>
+      <c r="K788" s="60"/>
+      <c r="L788" s="60"/>
+      <c r="M788" s="60"/>
+      <c r="N788" s="60"/>
+      <c r="O788" s="60"/>
+      <c r="P788" s="62"/>
     </row>
     <row r="789" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B789" s="5"/>
@@ -14628,46 +14626,46 @@
       <c r="P804" s="20"/>
     </row>
     <row r="805" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B805" s="61" t="s">
+      <c r="B805" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C805" s="62"/>
-      <c r="D805" s="62" t="s">
+      <c r="C805" s="58"/>
+      <c r="D805" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E805" s="62"/>
-      <c r="F805" s="62"/>
-      <c r="G805" s="65"/>
-      <c r="H805" s="67" t="s">
+      <c r="E805" s="58"/>
+      <c r="F805" s="58"/>
+      <c r="G805" s="61"/>
+      <c r="H805" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I805" s="62" t="s">
+      <c r="I805" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J805" s="62"/>
-      <c r="K805" s="62"/>
-      <c r="L805" s="62"/>
-      <c r="M805" s="62"/>
-      <c r="N805" s="62"/>
-      <c r="O805" s="62"/>
-      <c r="P805" s="65"/>
+      <c r="J805" s="58"/>
+      <c r="K805" s="58"/>
+      <c r="L805" s="58"/>
+      <c r="M805" s="58"/>
+      <c r="N805" s="58"/>
+      <c r="O805" s="58"/>
+      <c r="P805" s="61"/>
     </row>
     <row r="806" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B806" s="63"/>
-      <c r="C806" s="64"/>
-      <c r="D806" s="64"/>
-      <c r="E806" s="64"/>
-      <c r="F806" s="64"/>
-      <c r="G806" s="66"/>
-      <c r="H806" s="68"/>
-      <c r="I806" s="64"/>
-      <c r="J806" s="64"/>
-      <c r="K806" s="64"/>
-      <c r="L806" s="64"/>
-      <c r="M806" s="64"/>
-      <c r="N806" s="64"/>
-      <c r="O806" s="64"/>
-      <c r="P806" s="66"/>
+      <c r="B806" s="59"/>
+      <c r="C806" s="60"/>
+      <c r="D806" s="60"/>
+      <c r="E806" s="60"/>
+      <c r="F806" s="60"/>
+      <c r="G806" s="62"/>
+      <c r="H806" s="64"/>
+      <c r="I806" s="60"/>
+      <c r="J806" s="60"/>
+      <c r="K806" s="60"/>
+      <c r="L806" s="60"/>
+      <c r="M806" s="60"/>
+      <c r="N806" s="60"/>
+      <c r="O806" s="60"/>
+      <c r="P806" s="62"/>
     </row>
     <row r="807" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B807" s="5"/>
@@ -14917,46 +14915,46 @@
       <c r="P822" s="20"/>
     </row>
     <row r="823" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B823" s="61" t="s">
+      <c r="B823" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C823" s="62"/>
-      <c r="D823" s="62" t="s">
+      <c r="C823" s="58"/>
+      <c r="D823" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E823" s="62"/>
-      <c r="F823" s="62"/>
-      <c r="G823" s="65"/>
-      <c r="H823" s="67" t="s">
+      <c r="E823" s="58"/>
+      <c r="F823" s="58"/>
+      <c r="G823" s="61"/>
+      <c r="H823" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I823" s="62" t="s">
+      <c r="I823" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J823" s="62"/>
-      <c r="K823" s="62"/>
-      <c r="L823" s="62"/>
-      <c r="M823" s="62"/>
-      <c r="N823" s="62"/>
-      <c r="O823" s="62"/>
-      <c r="P823" s="65"/>
+      <c r="J823" s="58"/>
+      <c r="K823" s="58"/>
+      <c r="L823" s="58"/>
+      <c r="M823" s="58"/>
+      <c r="N823" s="58"/>
+      <c r="O823" s="58"/>
+      <c r="P823" s="61"/>
     </row>
     <row r="824" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B824" s="63"/>
-      <c r="C824" s="64"/>
-      <c r="D824" s="64"/>
-      <c r="E824" s="64"/>
-      <c r="F824" s="64"/>
-      <c r="G824" s="66"/>
-      <c r="H824" s="68"/>
-      <c r="I824" s="64"/>
-      <c r="J824" s="64"/>
-      <c r="K824" s="64"/>
-      <c r="L824" s="64"/>
-      <c r="M824" s="64"/>
-      <c r="N824" s="64"/>
-      <c r="O824" s="64"/>
-      <c r="P824" s="66"/>
+      <c r="B824" s="59"/>
+      <c r="C824" s="60"/>
+      <c r="D824" s="60"/>
+      <c r="E824" s="60"/>
+      <c r="F824" s="60"/>
+      <c r="G824" s="62"/>
+      <c r="H824" s="64"/>
+      <c r="I824" s="60"/>
+      <c r="J824" s="60"/>
+      <c r="K824" s="60"/>
+      <c r="L824" s="60"/>
+      <c r="M824" s="60"/>
+      <c r="N824" s="60"/>
+      <c r="O824" s="60"/>
+      <c r="P824" s="62"/>
     </row>
     <row r="825" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B825" s="5"/>
@@ -15206,46 +15204,46 @@
       <c r="P840" s="20"/>
     </row>
     <row r="841" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B841" s="61" t="s">
+      <c r="B841" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C841" s="62"/>
-      <c r="D841" s="62" t="s">
+      <c r="C841" s="58"/>
+      <c r="D841" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E841" s="62"/>
-      <c r="F841" s="62"/>
-      <c r="G841" s="65"/>
-      <c r="H841" s="67" t="s">
+      <c r="E841" s="58"/>
+      <c r="F841" s="58"/>
+      <c r="G841" s="61"/>
+      <c r="H841" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I841" s="62" t="s">
+      <c r="I841" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J841" s="62"/>
-      <c r="K841" s="62"/>
-      <c r="L841" s="62"/>
-      <c r="M841" s="62"/>
-      <c r="N841" s="62"/>
-      <c r="O841" s="62"/>
-      <c r="P841" s="65"/>
+      <c r="J841" s="58"/>
+      <c r="K841" s="58"/>
+      <c r="L841" s="58"/>
+      <c r="M841" s="58"/>
+      <c r="N841" s="58"/>
+      <c r="O841" s="58"/>
+      <c r="P841" s="61"/>
     </row>
     <row r="842" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B842" s="63"/>
-      <c r="C842" s="64"/>
-      <c r="D842" s="64"/>
-      <c r="E842" s="64"/>
-      <c r="F842" s="64"/>
-      <c r="G842" s="66"/>
-      <c r="H842" s="68"/>
-      <c r="I842" s="64"/>
-      <c r="J842" s="64"/>
-      <c r="K842" s="64"/>
-      <c r="L842" s="64"/>
-      <c r="M842" s="64"/>
-      <c r="N842" s="64"/>
-      <c r="O842" s="64"/>
-      <c r="P842" s="66"/>
+      <c r="B842" s="59"/>
+      <c r="C842" s="60"/>
+      <c r="D842" s="60"/>
+      <c r="E842" s="60"/>
+      <c r="F842" s="60"/>
+      <c r="G842" s="62"/>
+      <c r="H842" s="64"/>
+      <c r="I842" s="60"/>
+      <c r="J842" s="60"/>
+      <c r="K842" s="60"/>
+      <c r="L842" s="60"/>
+      <c r="M842" s="60"/>
+      <c r="N842" s="60"/>
+      <c r="O842" s="60"/>
+      <c r="P842" s="62"/>
     </row>
     <row r="843" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B843" s="5"/>
@@ -15495,46 +15493,46 @@
       <c r="P858" s="20"/>
     </row>
     <row r="859" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B859" s="61" t="s">
+      <c r="B859" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C859" s="62"/>
-      <c r="D859" s="62" t="s">
+      <c r="C859" s="58"/>
+      <c r="D859" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E859" s="62"/>
-      <c r="F859" s="62"/>
-      <c r="G859" s="65"/>
-      <c r="H859" s="67" t="s">
+      <c r="E859" s="58"/>
+      <c r="F859" s="58"/>
+      <c r="G859" s="61"/>
+      <c r="H859" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I859" s="62" t="s">
+      <c r="I859" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J859" s="62"/>
-      <c r="K859" s="62"/>
-      <c r="L859" s="62"/>
-      <c r="M859" s="62"/>
-      <c r="N859" s="62"/>
-      <c r="O859" s="62"/>
-      <c r="P859" s="65"/>
+      <c r="J859" s="58"/>
+      <c r="K859" s="58"/>
+      <c r="L859" s="58"/>
+      <c r="M859" s="58"/>
+      <c r="N859" s="58"/>
+      <c r="O859" s="58"/>
+      <c r="P859" s="61"/>
     </row>
     <row r="860" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B860" s="63"/>
-      <c r="C860" s="64"/>
-      <c r="D860" s="64"/>
-      <c r="E860" s="64"/>
-      <c r="F860" s="64"/>
-      <c r="G860" s="66"/>
-      <c r="H860" s="68"/>
-      <c r="I860" s="64"/>
-      <c r="J860" s="64"/>
-      <c r="K860" s="64"/>
-      <c r="L860" s="64"/>
-      <c r="M860" s="64"/>
-      <c r="N860" s="64"/>
-      <c r="O860" s="64"/>
-      <c r="P860" s="66"/>
+      <c r="B860" s="59"/>
+      <c r="C860" s="60"/>
+      <c r="D860" s="60"/>
+      <c r="E860" s="60"/>
+      <c r="F860" s="60"/>
+      <c r="G860" s="62"/>
+      <c r="H860" s="64"/>
+      <c r="I860" s="60"/>
+      <c r="J860" s="60"/>
+      <c r="K860" s="60"/>
+      <c r="L860" s="60"/>
+      <c r="M860" s="60"/>
+      <c r="N860" s="60"/>
+      <c r="O860" s="60"/>
+      <c r="P860" s="62"/>
     </row>
     <row r="861" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B861" s="5"/>
@@ -15784,46 +15782,46 @@
       <c r="P876" s="20"/>
     </row>
     <row r="877" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B877" s="61" t="s">
+      <c r="B877" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C877" s="62"/>
-      <c r="D877" s="62" t="s">
+      <c r="C877" s="58"/>
+      <c r="D877" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E877" s="62"/>
-      <c r="F877" s="62"/>
-      <c r="G877" s="65"/>
-      <c r="H877" s="67" t="s">
+      <c r="E877" s="58"/>
+      <c r="F877" s="58"/>
+      <c r="G877" s="61"/>
+      <c r="H877" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I877" s="62" t="s">
+      <c r="I877" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="J877" s="62"/>
-      <c r="K877" s="62"/>
-      <c r="L877" s="62"/>
-      <c r="M877" s="62"/>
-      <c r="N877" s="62"/>
-      <c r="O877" s="62"/>
-      <c r="P877" s="65"/>
+      <c r="J877" s="58"/>
+      <c r="K877" s="58"/>
+      <c r="L877" s="58"/>
+      <c r="M877" s="58"/>
+      <c r="N877" s="58"/>
+      <c r="O877" s="58"/>
+      <c r="P877" s="61"/>
     </row>
     <row r="878" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B878" s="63"/>
-      <c r="C878" s="64"/>
-      <c r="D878" s="64"/>
-      <c r="E878" s="64"/>
-      <c r="F878" s="64"/>
-      <c r="G878" s="66"/>
-      <c r="H878" s="68"/>
-      <c r="I878" s="64"/>
-      <c r="J878" s="64"/>
-      <c r="K878" s="64"/>
-      <c r="L878" s="64"/>
-      <c r="M878" s="64"/>
-      <c r="N878" s="64"/>
-      <c r="O878" s="64"/>
-      <c r="P878" s="66"/>
+      <c r="B878" s="59"/>
+      <c r="C878" s="60"/>
+      <c r="D878" s="60"/>
+      <c r="E878" s="60"/>
+      <c r="F878" s="60"/>
+      <c r="G878" s="62"/>
+      <c r="H878" s="64"/>
+      <c r="I878" s="60"/>
+      <c r="J878" s="60"/>
+      <c r="K878" s="60"/>
+      <c r="L878" s="60"/>
+      <c r="M878" s="60"/>
+      <c r="N878" s="60"/>
+      <c r="O878" s="60"/>
+      <c r="P878" s="62"/>
     </row>
     <row r="879" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B879" s="5"/>
@@ -16194,10 +16192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBB1695-5899-4647-9C9E-3DF62F447E3B}">
-  <dimension ref="A1:LN12"/>
+  <dimension ref="A1:LN6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16555,22 +16553,22 @@
       <c r="LN1" s="47"/>
     </row>
     <row r="2" spans="1:326" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="79">
+      <c r="A2" s="75">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="96" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="55" t="s">
@@ -16578,128 +16576,94 @@
       </c>
     </row>
     <row r="3" spans="1:326" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="60" t="s">
+      <c r="A3" s="75"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:326" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="75"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="95" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="96" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:326" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="78">
+        <v>2</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="102" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="102" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="102" t="s">
+      <c r="D5" s="96" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:326" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="79"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="101" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="102" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="102" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="55"/>
-    </row>
-    <row r="5" spans="1:326" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="83">
-        <v>2</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="84"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="84"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="84"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="55"/>
-    </row>
-    <row r="9" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="84"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="84"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="84"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="55"/>
-    </row>
-    <row r="12" spans="1:326" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="85"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="55"/>
+    <row r="6" spans="1:326" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="79"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="96" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{025F31CA-4A3A-BA43-BA45-0ABF2496162D}"/>
+  <autoFilter ref="A1:G6" xr:uid="{025F31CA-4A3A-BA43-BA45-0ABF2496162D}"/>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
-  <phoneticPr fontId="26" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -16763,7 +16727,7 @@
       </c>
     </row>
     <row r="11" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="86" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -16771,27 +16735,27 @@
       </c>
     </row>
     <row r="12" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="93"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="95"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="96"/>
-      <c r="D14" s="97"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="91"/>
     </row>
     <row r="15" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="98"/>
-      <c r="D15" s="99"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="93"/>
     </row>
     <row r="16" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="100" t="s">
+      <c r="C16" s="94" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -16799,27 +16763,27 @@
       </c>
     </row>
     <row r="17" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="93"/>
+      <c r="C17" s="87"/>
       <c r="D17" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="94" t="s">
+      <c r="C18" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="95"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="96"/>
-      <c r="D19" s="97"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="91"/>
     </row>
     <row r="20" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="93"/>
     </row>
     <row r="21" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="94" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="29" t="s">
@@ -16827,24 +16791,24 @@
       </c>
     </row>
     <row r="22" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="93"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="94" t="s">
+      <c r="C23" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="95"/>
+      <c r="D23" s="89"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="96"/>
-      <c r="D24" s="97"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="91"/>
     </row>
     <row r="25" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="98"/>
-      <c r="D25" s="99"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="93"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="30"/>
@@ -16930,26 +16894,26 @@
       <c r="D43" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="86" t="s">
+      <c r="E43" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="87"/>
+      <c r="F43" s="81"/>
     </row>
     <row r="44" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="36" t="s">
         <v>48</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="88"/>
-      <c r="F44" s="89"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="83"/>
     </row>
     <row r="45" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="36" t="s">
         <v>49</v>
       </c>
       <c r="D45" s="38"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="91"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>